<commit_message>
use last 5yr prices with RIN and rerun simulations for final publication
</commit_message>
<xml_diff>
--- a/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
+++ b/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
@@ -794,7 +794,7 @@
         <v>55</v>
       </c>
       <c r="C4">
-        <v>0.01296371811363718</v>
+        <v>0.0148164296321643</v>
       </c>
       <c r="D4">
         <v>0.00151221894312219</v>
@@ -803,31 +803,31 @@
         <v>0.01712925642329256</v>
       </c>
       <c r="G4">
-        <v>0.0006357176103571761</v>
+        <v>0.0006357038103570381</v>
       </c>
       <c r="I4">
         <v>0.0006457376344573764</v>
       </c>
       <c r="J4">
-        <v>0.00809015661856104</v>
+        <v>0.001873686026875668</v>
       </c>
       <c r="K4">
-        <v>-0.0007177648271776482</v>
+        <v>-0.0007194071231940713</v>
       </c>
       <c r="L4">
-        <v>-0.0007177648271776482</v>
+        <v>-0.0007194071231940713</v>
       </c>
       <c r="O4">
-        <v>-0.0007177648271776482</v>
+        <v>-0.0007194071231940713</v>
       </c>
       <c r="P4">
-        <v>-0.0006270437822704379</v>
+        <v>-0.0006269746742697467</v>
       </c>
       <c r="Q4">
-        <v>-0.0006921604869216049</v>
+        <v>-0.0006918716829187168</v>
       </c>
       <c r="R4">
-        <v>-0.0006921604869216049</v>
+        <v>-0.0006918716829187168</v>
       </c>
     </row>
     <row r="5" spans="1:31">
@@ -836,7 +836,7 @@
         <v>56</v>
       </c>
       <c r="C5">
-        <v>-0.003930489759304898</v>
+        <v>-0.005242748668427486</v>
       </c>
       <c r="D5">
         <v>0.0009778538137785381</v>
@@ -845,31 +845,31 @@
         <v>-0.01525117390451174</v>
       </c>
       <c r="G5">
-        <v>-0.002193366837933668</v>
+        <v>-0.002193411789934117</v>
       </c>
       <c r="I5">
         <v>-0.002392384391923844</v>
       </c>
       <c r="J5">
-        <v>0.0009696382330352183</v>
+        <v>-0.004755469532876422</v>
       </c>
       <c r="K5">
-        <v>0.002229759418297594</v>
+        <v>0.002231237686312377</v>
       </c>
       <c r="L5">
-        <v>0.002229759418297594</v>
+        <v>0.002231237686312377</v>
       </c>
       <c r="O5">
-        <v>0.002229759418297594</v>
+        <v>0.002231237686312377</v>
       </c>
       <c r="P5">
-        <v>0.002192825541928255</v>
+        <v>0.002192748081927481</v>
       </c>
       <c r="Q5">
-        <v>0.002206013806060138</v>
+        <v>0.002206465930064659</v>
       </c>
       <c r="R5">
-        <v>0.002206013806060138</v>
+        <v>0.002206465930064659</v>
       </c>
     </row>
     <row r="6" spans="1:31">
@@ -878,7 +878,7 @@
         <v>57</v>
       </c>
       <c r="C6">
-        <v>0.3251413542714136</v>
+        <v>0.2828656471286564</v>
       </c>
       <c r="D6">
         <v>-0.02621256331012563</v>
@@ -887,31 +887,31 @@
         <v>-0.492902494845025</v>
       </c>
       <c r="G6">
-        <v>-0.6208494281684942</v>
+        <v>-0.6208497665684977</v>
       </c>
       <c r="I6">
         <v>-0.6213371147013711</v>
       </c>
       <c r="J6">
-        <v>-0.006662209349307017</v>
+        <v>-0.000700843192824616</v>
       </c>
       <c r="K6">
-        <v>0.6208414599764146</v>
+        <v>0.6208431347804313</v>
       </c>
       <c r="L6">
-        <v>0.6208414599764146</v>
+        <v>0.6208431347804313</v>
       </c>
       <c r="O6">
-        <v>0.6208414599764146</v>
+        <v>0.6208431347804313</v>
       </c>
       <c r="P6">
-        <v>0.6208520935845209</v>
+        <v>0.620852303200523</v>
       </c>
       <c r="Q6">
-        <v>0.6208394239243942</v>
+        <v>0.6208391764843918</v>
       </c>
       <c r="R6">
-        <v>0.6208394239243942</v>
+        <v>0.6208391764843918</v>
       </c>
     </row>
     <row r="7" spans="1:31">
@@ -920,7 +920,7 @@
         <v>58</v>
       </c>
       <c r="C7">
-        <v>0.009436487278364873</v>
+        <v>0.01030776876707769</v>
       </c>
       <c r="D7">
         <v>0.02194901197549012</v>
@@ -929,31 +929,31 @@
         <v>0.02374809681348097</v>
       </c>
       <c r="G7">
-        <v>0.02247280892072809</v>
+        <v>0.02247264428072644</v>
       </c>
       <c r="I7">
         <v>0.02254483872944839</v>
       </c>
       <c r="J7">
-        <v>0.01589339824295197</v>
+        <v>0.009543290109709992</v>
       </c>
       <c r="K7">
-        <v>-0.02249685917696859</v>
+        <v>-0.02250033418500334</v>
       </c>
       <c r="L7">
-        <v>-0.02249685917696859</v>
+        <v>-0.02250033418500334</v>
       </c>
       <c r="O7">
-        <v>-0.02249685917696859</v>
+        <v>-0.02250033418500334</v>
       </c>
       <c r="P7">
-        <v>-0.02247366497673665</v>
+        <v>-0.02247407370874074</v>
       </c>
       <c r="Q7">
-        <v>-0.0224874205768742</v>
+        <v>-0.02248712856887129</v>
       </c>
       <c r="R7">
-        <v>-0.0224874205768742</v>
+        <v>-0.02248712856887129</v>
       </c>
     </row>
     <row r="8" spans="1:31">
@@ -962,7 +962,7 @@
         <v>59</v>
       </c>
       <c r="C8">
-        <v>0.3117376833693769</v>
+        <v>0.2684335947083359</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -971,31 +971,31 @@
         <v>0.6224610370166104</v>
       </c>
       <c r="G8">
-        <v>0.7875800424758005</v>
+        <v>0.7875797851957979</v>
       </c>
       <c r="I8">
         <v>0.787382098681821</v>
       </c>
       <c r="J8">
-        <v>0.009090273761515359</v>
+        <v>-6.668716596108231E-05</v>
       </c>
       <c r="K8">
-        <v>-0.7875837780758378</v>
+        <v>-0.7875819821558198</v>
       </c>
       <c r="L8">
-        <v>-0.7875837780758378</v>
+        <v>-0.7875819821558198</v>
       </c>
       <c r="O8">
-        <v>-0.7875837780758378</v>
+        <v>-0.7875819821558198</v>
       </c>
       <c r="P8">
-        <v>-0.7875769787317699</v>
+        <v>-0.787576802535768</v>
       </c>
       <c r="Q8">
-        <v>-0.7875887595038876</v>
+        <v>-0.7875889731038898</v>
       </c>
       <c r="R8">
-        <v>-0.7875887595038876</v>
+        <v>-0.7875889731038898</v>
       </c>
     </row>
     <row r="9" spans="1:31">
@@ -1006,7 +1006,7 @@
         <v>60</v>
       </c>
       <c r="C9">
-        <v>-0.005225322892253229</v>
+        <v>-0.004327833211278332</v>
       </c>
       <c r="D9">
         <v>-0.009849915098499151</v>
@@ -1015,31 +1015,31 @@
         <v>-0.005273047624730476</v>
       </c>
       <c r="G9">
-        <v>-0.0008174110281741103</v>
+        <v>-0.0008179209441792094</v>
       </c>
       <c r="I9">
         <v>-0.0003577986275779863</v>
       </c>
       <c r="J9">
-        <v>-0.03362173557571643</v>
+        <v>-0.004876688950829339</v>
       </c>
       <c r="K9">
-        <v>0.0008296441402964414</v>
+        <v>0.0008287248802872489</v>
       </c>
       <c r="L9">
-        <v>0.0008296441402964414</v>
+        <v>0.0008287248802872489</v>
       </c>
       <c r="O9">
-        <v>0.0008296441402964414</v>
+        <v>0.0008287248802872489</v>
       </c>
       <c r="P9">
-        <v>0.0008104499001044991</v>
+        <v>0.0008103354921033551</v>
       </c>
       <c r="Q9">
-        <v>0.0008343581243435813</v>
+        <v>0.0008343521123435211</v>
       </c>
       <c r="R9">
-        <v>0.0008343581243435813</v>
+        <v>0.0008343521123435211</v>
       </c>
     </row>
     <row r="10" spans="1:31">
@@ -1050,7 +1050,7 @@
         <v>60</v>
       </c>
       <c r="C10">
-        <v>0.7582480644944807</v>
+        <v>0.8240005612520057</v>
       </c>
       <c r="D10">
         <v>-0.006061106124611061</v>
@@ -1059,31 +1059,31 @@
         <v>-0.009698970816989708</v>
       </c>
       <c r="G10">
-        <v>-0.0113697704096977</v>
+        <v>-0.01136968310969683</v>
       </c>
       <c r="I10">
         <v>-0.01126867538868675</v>
       </c>
       <c r="J10">
-        <v>-0.005149363275088247</v>
+        <v>-0.01583476228550769</v>
       </c>
       <c r="K10">
-        <v>0.01138806926988069</v>
+        <v>0.01138975754989758</v>
       </c>
       <c r="L10">
-        <v>0.01138806926988069</v>
+        <v>0.01138975754989758</v>
       </c>
       <c r="O10">
-        <v>0.01138806926988069</v>
+        <v>0.01138975754989758</v>
       </c>
       <c r="P10">
-        <v>0.01137316735773167</v>
+        <v>0.01137315092973151</v>
       </c>
       <c r="Q10">
-        <v>0.01138818840588188</v>
+        <v>0.0113882702578827</v>
       </c>
       <c r="R10">
-        <v>0.01138818840588188</v>
+        <v>0.0113882702578827</v>
       </c>
     </row>
     <row r="11" spans="1:31">
@@ -1094,7 +1094,7 @@
         <v>60</v>
       </c>
       <c r="C11">
-        <v>0.001324978873249789</v>
+        <v>0.001205539308055393</v>
       </c>
       <c r="D11">
         <v>-1.081171210811712E-05</v>
@@ -1103,31 +1103,31 @@
         <v>0.01481179351611794</v>
       </c>
       <c r="G11">
-        <v>0.004688577202885772</v>
+        <v>0.00468864202688642</v>
       </c>
       <c r="I11">
         <v>0.004428350672283508</v>
       </c>
       <c r="J11">
-        <v>-0.0007062620015870604</v>
+        <v>-0.01407036079278574</v>
       </c>
       <c r="K11">
-        <v>-0.004777976555779765</v>
+        <v>-0.004781005403810054</v>
       </c>
       <c r="L11">
-        <v>-0.004777976555779765</v>
+        <v>-0.004781005403810054</v>
       </c>
       <c r="O11">
-        <v>-0.004777976555779765</v>
+        <v>-0.004781005403810054</v>
       </c>
       <c r="P11">
-        <v>-0.004677035710770357</v>
+        <v>-0.004677374842773749</v>
       </c>
       <c r="Q11">
-        <v>-0.004737853139378531</v>
+        <v>-0.004738099379380994</v>
       </c>
       <c r="R11">
-        <v>-0.004737853139378531</v>
+        <v>-0.004738099379380994</v>
       </c>
     </row>
     <row r="12" spans="1:31">
@@ -1138,7 +1138,7 @@
         <v>61</v>
       </c>
       <c r="C12">
-        <v>0.02345885455858855</v>
+        <v>0.02266218575862185</v>
       </c>
       <c r="D12">
         <v>0.01840892352408923</v>
@@ -1147,31 +1147,31 @@
         <v>0.006248929538489295</v>
       </c>
       <c r="G12">
-        <v>0.01013825759338258</v>
+        <v>0.01013836278538363</v>
       </c>
       <c r="I12">
         <v>0.01012691094526911</v>
       </c>
       <c r="J12">
-        <v>0.01183566166533927</v>
+        <v>0.0004537099816154965</v>
       </c>
       <c r="K12">
-        <v>-0.01014076625340766</v>
+        <v>-0.01014380634543806</v>
       </c>
       <c r="L12">
-        <v>-0.01014076625340766</v>
+        <v>-0.01014380634543806</v>
       </c>
       <c r="O12">
-        <v>-0.01014076625340766</v>
+        <v>-0.01014380634543806</v>
       </c>
       <c r="P12">
-        <v>-0.01013562835735628</v>
+        <v>-0.01013550437335504</v>
       </c>
       <c r="Q12">
-        <v>-0.01013653193336532</v>
+        <v>-0.01013627480936275</v>
       </c>
       <c r="R12">
-        <v>-0.01013653193336532</v>
+        <v>-0.01013627480936275</v>
       </c>
     </row>
     <row r="13" spans="1:31">
@@ -1182,7 +1182,7 @@
         <v>62</v>
       </c>
       <c r="C13">
-        <v>0.05662474020224741</v>
+        <v>0.05010769224907692</v>
       </c>
       <c r="D13">
         <v>-0.02004360854043609</v>
@@ -1191,31 +1191,31 @@
         <v>-0.007983215575832156</v>
       </c>
       <c r="G13">
-        <v>-0.008684091794840918</v>
+        <v>-0.008683869242838692</v>
       </c>
       <c r="I13">
         <v>-0.008591242561912425</v>
       </c>
       <c r="J13">
-        <v>0.00784250866989937</v>
+        <v>0.009259240951473371</v>
       </c>
       <c r="K13">
-        <v>0.008686992422869924</v>
+        <v>0.008689972202899724</v>
       </c>
       <c r="L13">
-        <v>0.008686992422869924</v>
+        <v>0.008689972202899724</v>
       </c>
       <c r="O13">
-        <v>0.008686992422869924</v>
+        <v>0.008689972202899724</v>
       </c>
       <c r="P13">
-        <v>0.008677381346773814</v>
+        <v>0.0086772297987723</v>
       </c>
       <c r="Q13">
-        <v>0.008688997766889977</v>
+        <v>0.008689141202891413</v>
       </c>
       <c r="R13">
-        <v>0.008688997766889977</v>
+        <v>0.008689141202891413</v>
       </c>
     </row>
     <row r="14" spans="1:31">
@@ -1224,7 +1224,7 @@
         <v>63</v>
       </c>
       <c r="C14">
-        <v>-0.410485303116853</v>
+        <v>-0.3542953498709535</v>
       </c>
       <c r="D14">
         <v>-0.003031562910315629</v>
@@ -1233,31 +1233,31 @@
         <v>-0.0125199202251992</v>
       </c>
       <c r="G14">
-        <v>-0.0138999895389999</v>
+        <v>-0.01390005859900059</v>
       </c>
       <c r="I14">
         <v>-0.01418066613380666</v>
       </c>
       <c r="J14">
-        <v>-0.008801855070386055</v>
+        <v>0.001565608492603544</v>
       </c>
       <c r="K14">
-        <v>0.01392420714724207</v>
+        <v>0.01392549905525499</v>
       </c>
       <c r="L14">
-        <v>0.01392420714724207</v>
+        <v>0.01392549905525499</v>
       </c>
       <c r="O14">
-        <v>0.01392420714724207</v>
+        <v>0.01392549905525499</v>
       </c>
       <c r="P14">
-        <v>0.01389505651895056</v>
+        <v>0.01389444315094443</v>
       </c>
       <c r="Q14">
-        <v>0.01391906439119065</v>
+        <v>0.01391916102719161</v>
       </c>
       <c r="R14">
-        <v>0.01391906439119065</v>
+        <v>0.01391916102719161</v>
       </c>
     </row>
     <row r="15" spans="1:31">
@@ -1268,7 +1268,7 @@
         <v>64</v>
       </c>
       <c r="C15">
-        <v>0.001853512110535121</v>
+        <v>0.00107900095079001</v>
       </c>
       <c r="D15">
         <v>-0.002824025776240258</v>
@@ -1277,31 +1277,31 @@
         <v>-0.004522843185228432</v>
       </c>
       <c r="G15">
-        <v>-0.00667376788273768</v>
+        <v>-0.006673683882736838</v>
       </c>
       <c r="I15">
         <v>-0.006586563185865632</v>
       </c>
       <c r="J15">
-        <v>0.01414130437897065</v>
+        <v>0.01015344027457751</v>
       </c>
       <c r="K15">
-        <v>0.006664717482647175</v>
+        <v>0.006667343538673435</v>
       </c>
       <c r="L15">
-        <v>0.006664717482647175</v>
+        <v>0.006667343538673435</v>
       </c>
       <c r="O15">
-        <v>0.006664717482647175</v>
+        <v>0.006667343538673435</v>
       </c>
       <c r="P15">
-        <v>0.006675425226754251</v>
+        <v>0.006675547566755476</v>
       </c>
       <c r="Q15">
-        <v>0.006664126350641263</v>
+        <v>0.006663872346638724</v>
       </c>
       <c r="R15">
-        <v>0.006664126350641263</v>
+        <v>0.006663872346638724</v>
       </c>
     </row>
     <row r="16" spans="1:31">
@@ -1312,7 +1312,7 @@
         <v>64</v>
       </c>
       <c r="C16">
-        <v>-0.006059043732590437</v>
+        <v>-0.007867395522673955</v>
       </c>
       <c r="D16">
         <v>0.0007758225677582258</v>
@@ -1321,31 +1321,31 @@
         <v>-0.002102966469029665</v>
       </c>
       <c r="G16">
-        <v>-0.001062989902629899</v>
+        <v>-0.001063054462630545</v>
       </c>
       <c r="I16">
         <v>-0.0008461253484612535</v>
       </c>
       <c r="J16">
-        <v>-0.007001960695954742</v>
+        <v>-0.008438939242291991</v>
       </c>
       <c r="K16">
-        <v>0.001029366094293661</v>
+        <v>0.001033075906330759</v>
       </c>
       <c r="L16">
-        <v>0.001029366094293661</v>
+        <v>0.001033075906330759</v>
       </c>
       <c r="O16">
-        <v>0.001029366094293661</v>
+        <v>0.001033075906330759</v>
       </c>
       <c r="P16">
-        <v>0.001065465778654658</v>
+        <v>0.001065458734654587</v>
       </c>
       <c r="Q16">
-        <v>0.001046041534460415</v>
+        <v>0.001046190742461908</v>
       </c>
       <c r="R16">
-        <v>0.001046041534460415</v>
+        <v>0.001046190742461908</v>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -1356,7 +1356,7 @@
         <v>65</v>
       </c>
       <c r="C17">
-        <v>0.01269746226697462</v>
+        <v>0.01014700625347006</v>
       </c>
       <c r="D17">
         <v>0.01176501519365015</v>
@@ -1365,31 +1365,31 @@
         <v>-0.002081501528815015</v>
       </c>
       <c r="G17">
-        <v>-0.004309387159093871</v>
+        <v>-0.004309450759094508</v>
       </c>
       <c r="I17">
         <v>-0.004342034131420341</v>
       </c>
       <c r="J17">
-        <v>-0.006633541991395263</v>
+        <v>0.007058441736929497</v>
       </c>
       <c r="K17">
-        <v>0.004308099331080993</v>
+        <v>0.004306603375066035</v>
       </c>
       <c r="L17">
-        <v>0.004308099331080993</v>
+        <v>0.004306603375066035</v>
       </c>
       <c r="O17">
-        <v>0.004308099331080993</v>
+        <v>0.004306603375066035</v>
       </c>
       <c r="P17">
-        <v>0.004311125131111251</v>
+        <v>0.004311253795112538</v>
       </c>
       <c r="Q17">
-        <v>0.004312297675122976</v>
+        <v>0.004312354567123546</v>
       </c>
       <c r="R17">
-        <v>0.004312297675122976</v>
+        <v>0.004312354567123546</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -1400,7 +1400,7 @@
         <v>64</v>
       </c>
       <c r="C18">
-        <v>0.00931432911314329</v>
+        <v>0.009169314655693147</v>
       </c>
       <c r="D18">
         <v>-0.001414514918145149</v>
@@ -1409,31 +1409,31 @@
         <v>-0.001909786711097867</v>
       </c>
       <c r="G18">
-        <v>-0.005818123450181234</v>
+        <v>-0.00581824093018241</v>
       </c>
       <c r="I18">
         <v>-0.005864057662640577</v>
       </c>
       <c r="J18">
-        <v>-0.008434552272117929</v>
+        <v>-0.01738753261916367</v>
       </c>
       <c r="K18">
-        <v>0.005804256670042567</v>
+        <v>0.005802721726027218</v>
       </c>
       <c r="L18">
-        <v>0.005804256670042567</v>
+        <v>0.005802721726027218</v>
       </c>
       <c r="O18">
-        <v>0.005804256670042567</v>
+        <v>0.005802721726027218</v>
       </c>
       <c r="P18">
-        <v>0.005820569506205695</v>
+        <v>0.005820913306209132</v>
       </c>
       <c r="Q18">
-        <v>0.005822839138228391</v>
+        <v>0.005822729290227292</v>
       </c>
       <c r="R18">
-        <v>0.005822839138228391</v>
+        <v>0.005822729290227292</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -1442,7 +1442,7 @@
         <v>66</v>
       </c>
       <c r="C19">
-        <v>0.01648181061281811</v>
+        <v>0.01459265887392659</v>
       </c>
       <c r="D19">
         <v>0.01707790277077903</v>
@@ -1451,31 +1451,31 @@
         <v>0.00673844303538443</v>
       </c>
       <c r="G19">
-        <v>0.002647272842472728</v>
+        <v>0.002646988082469881</v>
       </c>
       <c r="I19">
         <v>0.0026238800422388</v>
       </c>
       <c r="J19">
-        <v>-0.008052698220710426</v>
+        <v>0.01521541544582149</v>
       </c>
       <c r="K19">
-        <v>-0.00263253301432533</v>
+        <v>-0.002631095714310957</v>
       </c>
       <c r="L19">
-        <v>-0.00263253301432533</v>
+        <v>-0.002631095714310957</v>
       </c>
       <c r="O19">
-        <v>-0.00263253301432533</v>
+        <v>-0.002631095714310957</v>
       </c>
       <c r="P19">
-        <v>-0.002652434702524347</v>
+        <v>-0.002652283466522835</v>
       </c>
       <c r="Q19">
-        <v>-0.002632186754321867</v>
+        <v>-0.002632375826323758</v>
       </c>
       <c r="R19">
-        <v>-0.002632186754321867</v>
+        <v>-0.002632375826323758</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -1486,7 +1486,7 @@
         <v>67</v>
       </c>
       <c r="C20">
-        <v>-0.006769798483697985</v>
+        <v>-0.006772085455720854</v>
       </c>
       <c r="D20">
         <v>-0.007641676312416763</v>
@@ -1495,31 +1495,31 @@
         <v>-0.01275603319956033</v>
       </c>
       <c r="G20">
-        <v>-0.01273861195938612</v>
+        <v>-0.01273863918738639</v>
       </c>
       <c r="I20">
         <v>-0.01277064880370649</v>
       </c>
       <c r="J20">
-        <v>0.002492884536847331</v>
+        <v>-0.0246030375246055</v>
       </c>
       <c r="K20">
-        <v>0.01279376938393769</v>
+        <v>0.01279567872795679</v>
       </c>
       <c r="L20">
-        <v>0.01279376938393769</v>
+        <v>0.01279567872795679</v>
       </c>
       <c r="O20">
-        <v>0.01279376938393769</v>
+        <v>0.01279567872795679</v>
       </c>
       <c r="P20">
-        <v>0.01273906747939067</v>
+        <v>0.01273885110738851</v>
       </c>
       <c r="Q20">
-        <v>0.01276632100366321</v>
+        <v>0.01276613907166139</v>
       </c>
       <c r="R20">
-        <v>0.01276632100366321</v>
+        <v>0.01276613907166139</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -1530,7 +1530,7 @@
         <v>68</v>
       </c>
       <c r="C21">
-        <v>-0.0004005515800055158</v>
+        <v>-0.001864848102648481</v>
       </c>
       <c r="D21">
         <v>0.004832216064322161</v>
@@ -1539,31 +1539,31 @@
         <v>0.008761591539615915</v>
       </c>
       <c r="G21">
-        <v>0.01026764949067649</v>
+        <v>0.01026772164667722</v>
       </c>
       <c r="I21">
         <v>0.01016340810563408</v>
       </c>
       <c r="J21">
-        <v>0.008504949053867767</v>
+        <v>0.004325829066586761</v>
       </c>
       <c r="K21">
-        <v>-0.01025879705458797</v>
+        <v>-0.01026386850663868</v>
       </c>
       <c r="L21">
-        <v>-0.01025879705458797</v>
+        <v>-0.01026386850663868</v>
       </c>
       <c r="O21">
-        <v>-0.01025879705458797</v>
+        <v>-0.01026386850663868</v>
       </c>
       <c r="P21">
-        <v>-0.01027035880270359</v>
+        <v>-0.01027046449870465</v>
       </c>
       <c r="Q21">
-        <v>-0.01026403123864031</v>
+        <v>-0.01026454063864541</v>
       </c>
       <c r="R21">
-        <v>-0.01026403123864031</v>
+        <v>-0.01026454063864541</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -1572,7 +1572,7 @@
         <v>69</v>
       </c>
       <c r="C22">
-        <v>-0.01681673656816737</v>
+        <v>-0.01586492279064923</v>
       </c>
       <c r="D22">
         <v>-7.972794079727941E-05</v>
@@ -1581,31 +1581,31 @@
         <v>0.02701235296212353</v>
       </c>
       <c r="G22">
-        <v>0.01163386932833869</v>
+        <v>0.01163395396433954</v>
       </c>
       <c r="I22">
         <v>0.01163227119232271</v>
       </c>
       <c r="J22">
-        <v>-0.009972968017463975</v>
+        <v>0.008407619532811611</v>
       </c>
       <c r="K22">
-        <v>-0.01174918210549182</v>
+        <v>-0.01175150354151503</v>
       </c>
       <c r="L22">
-        <v>-0.01174918210549182</v>
+        <v>-0.01175150354151503</v>
       </c>
       <c r="O22">
-        <v>-0.01174918210549182</v>
+        <v>-0.01175150354151503</v>
       </c>
       <c r="P22">
-        <v>-0.01162178878421789</v>
+        <v>-0.01162198329221983</v>
       </c>
       <c r="Q22">
-        <v>-0.01170338561703386</v>
+        <v>-0.01170356445303565</v>
       </c>
       <c r="R22">
-        <v>-0.01170338561703386</v>
+        <v>-0.01170356445303565</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -1614,7 +1614,7 @@
         <v>70</v>
       </c>
       <c r="C23">
-        <v>0.01073153693931537</v>
+        <v>0.01001863292818633</v>
       </c>
       <c r="D23">
         <v>0.01001911825619118</v>
@@ -1623,31 +1623,31 @@
         <v>0.007504299915042999</v>
       </c>
       <c r="G23">
-        <v>-0.002178959373789594</v>
+        <v>-0.002179117089791171</v>
       </c>
       <c r="I23">
         <v>-0.002599315189993152</v>
       </c>
       <c r="J23">
-        <v>-0.01259674634244373</v>
+        <v>-0.008192914276423557</v>
       </c>
       <c r="K23">
-        <v>0.002094094904940949</v>
+        <v>0.002088460628884606</v>
       </c>
       <c r="L23">
-        <v>0.002094094904940949</v>
+        <v>0.002088460628884606</v>
       </c>
       <c r="O23">
-        <v>0.002094094904940949</v>
+        <v>0.002088460628884606</v>
       </c>
       <c r="P23">
-        <v>0.002176807857768079</v>
+        <v>0.00217650399376504</v>
       </c>
       <c r="Q23">
-        <v>0.002123592705235927</v>
+        <v>0.002123430189234302</v>
       </c>
       <c r="R23">
-        <v>0.002123592705235927</v>
+        <v>0.002123430189234302</v>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -1656,7 +1656,7 @@
         <v>71</v>
       </c>
       <c r="C24">
-        <v>-0.006042534108425341</v>
+        <v>-0.00610967290909673</v>
       </c>
       <c r="D24">
         <v>-0.01110188474701885</v>
@@ -1665,31 +1665,31 @@
         <v>-0.0153320895453209</v>
       </c>
       <c r="G24">
-        <v>-0.01419721168597212</v>
+        <v>-0.01419712702597127</v>
       </c>
       <c r="I24">
         <v>-0.01401925282419253</v>
       </c>
       <c r="J24">
-        <v>-0.002330458826073247</v>
+        <v>0.005401212400257207</v>
       </c>
       <c r="K24">
-        <v>0.01422355609023556</v>
+        <v>0.0142294406382944</v>
       </c>
       <c r="L24">
-        <v>0.01422355609023556</v>
+        <v>0.0142294406382944</v>
       </c>
       <c r="O24">
-        <v>0.01422355609023556</v>
+        <v>0.0142294406382944</v>
       </c>
       <c r="P24">
-        <v>0.01419004887390049</v>
+        <v>0.01419045251790452</v>
       </c>
       <c r="Q24">
-        <v>0.01421884640218847</v>
+        <v>0.01421851195018512</v>
       </c>
       <c r="R24">
-        <v>0.01421884640218847</v>
+        <v>0.01421851195018512</v>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -1700,7 +1700,7 @@
         <v>72</v>
       </c>
       <c r="C25">
-        <v>-0.001020961498209615</v>
+        <v>-0.001126837331268374</v>
       </c>
       <c r="D25">
         <v>0.001704990857049909</v>
@@ -1709,31 +1709,31 @@
         <v>-0.001873821138738211</v>
       </c>
       <c r="G25">
-        <v>-0.002629683578296836</v>
+        <v>-0.00262980297829803</v>
       </c>
       <c r="I25">
         <v>-0.00269752502697525</v>
       </c>
       <c r="J25">
-        <v>0.01030892623563578</v>
+        <v>0.009899400990695362</v>
       </c>
       <c r="K25">
-        <v>0.002622591746225918</v>
+        <v>0.002623444886234449</v>
       </c>
       <c r="L25">
-        <v>0.002622591746225918</v>
+        <v>0.002623444886234449</v>
       </c>
       <c r="O25">
-        <v>0.002622591746225918</v>
+        <v>0.002623444886234449</v>
       </c>
       <c r="P25">
-        <v>0.002633490206334902</v>
+        <v>0.002633286158332862</v>
       </c>
       <c r="Q25">
-        <v>0.00263035807430358</v>
+        <v>0.002630777474307775</v>
       </c>
       <c r="R25">
-        <v>0.00263035807430358</v>
+        <v>0.002630777474307775</v>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -1742,7 +1742,7 @@
         <v>73</v>
       </c>
       <c r="C26">
-        <v>0.01417445927774459</v>
+        <v>0.01545045230250452</v>
       </c>
       <c r="D26">
         <v>-0.01081725564017256</v>
@@ -1751,31 +1751,31 @@
         <v>-0.02193400050334001</v>
       </c>
       <c r="G26">
-        <v>-0.01488171590881716</v>
+        <v>-0.01488172783681728</v>
       </c>
       <c r="I26">
         <v>-0.0150762303067623</v>
       </c>
       <c r="J26">
-        <v>0.006527147993637605</v>
+        <v>-0.02005703061303707</v>
       </c>
       <c r="K26">
-        <v>0.01494788249347882</v>
+        <v>0.01495130618951306</v>
       </c>
       <c r="L26">
-        <v>0.01494788249347882</v>
+        <v>0.01495130618951306</v>
       </c>
       <c r="O26">
-        <v>0.01494788249347882</v>
+        <v>0.01495130618951306</v>
       </c>
       <c r="P26">
-        <v>0.01487519076475191</v>
+        <v>0.0148752400727524</v>
       </c>
       <c r="Q26">
-        <v>0.01491692257716923</v>
+        <v>0.01491661050516611</v>
       </c>
       <c r="R26">
-        <v>0.01491692257716923</v>
+        <v>0.01491661050516611</v>
       </c>
     </row>
     <row r="27" spans="1:18">
@@ -1786,7 +1786,7 @@
         <v>74</v>
       </c>
       <c r="C27">
-        <v>0.003310115265101153</v>
+        <v>0.003098167050981671</v>
       </c>
       <c r="D27">
         <v>-0.001261675212616752</v>
@@ -1795,31 +1795,31 @@
         <v>-0.006484291600842916</v>
       </c>
       <c r="G27">
-        <v>-0.002727241263272413</v>
+        <v>-0.00272717699127177</v>
       </c>
       <c r="I27">
         <v>-0.002869706212697062</v>
       </c>
       <c r="J27">
-        <v>0.002978842692440157</v>
+        <v>-0.01790454949168588</v>
       </c>
       <c r="K27">
-        <v>0.002767632771676328</v>
+        <v>0.002768992671689926</v>
       </c>
       <c r="L27">
-        <v>0.002767632771676328</v>
+        <v>0.002768992671689926</v>
       </c>
       <c r="O27">
-        <v>0.002767632771676328</v>
+        <v>0.002768992671689926</v>
       </c>
       <c r="P27">
-        <v>0.002723677131236771</v>
+        <v>0.002723668899236689</v>
       </c>
       <c r="Q27">
-        <v>0.00274256802342568</v>
+        <v>0.002742690819426909</v>
       </c>
       <c r="R27">
-        <v>0.00274256802342568</v>
+        <v>0.002742690819426909</v>
       </c>
     </row>
     <row r="28" spans="1:18">
@@ -1828,7 +1828,7 @@
         <v>75</v>
       </c>
       <c r="C28">
-        <v>0.001053793210537932</v>
+        <v>-0.0009040174890401748</v>
       </c>
       <c r="D28">
         <v>0.01474209685542097</v>
@@ -1837,31 +1837,31 @@
         <v>-0.0002166517941665179</v>
       </c>
       <c r="G28">
-        <v>0.003176749339767493</v>
+        <v>0.003176748415767484</v>
       </c>
       <c r="I28">
         <v>0.003240781484407815</v>
       </c>
       <c r="J28">
-        <v>0.006232893288185666</v>
+        <v>-0.0007549402438115624</v>
       </c>
       <c r="K28">
-        <v>-0.003163090603630906</v>
+        <v>-0.003162592063625921</v>
       </c>
       <c r="L28">
-        <v>-0.003163090603630906</v>
+        <v>-0.003162592063625921</v>
       </c>
       <c r="O28">
-        <v>-0.003163090603630906</v>
+        <v>-0.003162592063625921</v>
       </c>
       <c r="P28">
-        <v>-0.003170813227708132</v>
+        <v>-0.003170627707706277</v>
       </c>
       <c r="Q28">
-        <v>-0.003172702795727028</v>
+        <v>-0.003172870267728703</v>
       </c>
       <c r="R28">
-        <v>-0.003172702795727028</v>
+        <v>-0.003172870267728703</v>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -1872,7 +1872,7 @@
         <v>76</v>
       </c>
       <c r="C29">
-        <v>0.005234300560343005</v>
+        <v>0.006421504540215046</v>
       </c>
       <c r="D29">
         <v>-0.005577593131775931</v>
@@ -1881,31 +1881,31 @@
         <v>0.003891395678913957</v>
       </c>
       <c r="G29">
-        <v>0.001618015156180151</v>
+        <v>0.001618482664184827</v>
       </c>
       <c r="I29">
         <v>0.001829390214293902</v>
       </c>
       <c r="J29">
-        <v>-0.005647990317291082</v>
+        <v>0.002736921514177506</v>
       </c>
       <c r="K29">
-        <v>-0.001662942652629426</v>
+        <v>-0.001665123292651233</v>
       </c>
       <c r="L29">
-        <v>-0.001662942652629426</v>
+        <v>-0.001665123292651233</v>
       </c>
       <c r="O29">
-        <v>-0.001662942652629426</v>
+        <v>-0.001665123292651233</v>
       </c>
       <c r="P29">
-        <v>-0.001613229400132294</v>
+        <v>-0.001613021860130218</v>
       </c>
       <c r="Q29">
-        <v>-0.001639662412396624</v>
+        <v>-0.001639257532392575</v>
       </c>
       <c r="R29">
-        <v>-0.001639662412396624</v>
+        <v>-0.001639257532392575</v>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -1916,7 +1916,7 @@
         <v>77</v>
       </c>
       <c r="C30">
-        <v>-0.01068744321487443</v>
+        <v>-0.01095548902955489</v>
       </c>
       <c r="D30">
         <v>0.004842115728421158</v>
@@ -1925,31 +1925,31 @@
         <v>-0.006923286321232863</v>
       </c>
       <c r="G30">
-        <v>0.001799118833991188</v>
+        <v>0.001798965221989652</v>
       </c>
       <c r="I30">
         <v>0.001994068219940683</v>
       </c>
       <c r="J30">
-        <v>0.007914904916270494</v>
+        <v>0.007036224922380164</v>
       </c>
       <c r="K30">
-        <v>-0.001718718401187184</v>
+        <v>-0.001716728765167288</v>
       </c>
       <c r="L30">
-        <v>-0.001718718401187184</v>
+        <v>-0.001716728765167288</v>
       </c>
       <c r="O30">
-        <v>-0.001718718401187184</v>
+        <v>-0.001716728765167288</v>
       </c>
       <c r="P30">
-        <v>-0.001808951826089518</v>
+        <v>-0.001809245262092453</v>
       </c>
       <c r="Q30">
-        <v>-0.001752235817522358</v>
+        <v>-0.001752439073524391</v>
       </c>
       <c r="R30">
-        <v>-0.001752235817522358</v>
+        <v>-0.001752439073524391</v>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -1960,7 +1960,7 @@
         <v>78</v>
       </c>
       <c r="C31">
-        <v>-0.006916078893160789</v>
+        <v>-0.005876753866767539</v>
       </c>
       <c r="D31">
         <v>-0.01621171205411712</v>
@@ -1969,31 +1969,31 @@
         <v>-0.01224104058241041</v>
       </c>
       <c r="G31">
-        <v>-0.007624453336244534</v>
+        <v>-0.007624794412247945</v>
       </c>
       <c r="I31">
         <v>-0.007566174627661747</v>
       </c>
       <c r="J31">
-        <v>0.006890723575361845</v>
+        <v>-0.007177086466493077</v>
       </c>
       <c r="K31">
-        <v>0.007643956684439567</v>
+        <v>0.007643394604433947</v>
       </c>
       <c r="L31">
-        <v>0.007643956684439567</v>
+        <v>0.007643394604433947</v>
       </c>
       <c r="O31">
-        <v>0.007643956684439567</v>
+        <v>0.007643394604433947</v>
       </c>
       <c r="P31">
-        <v>0.007617235612172356</v>
+        <v>0.007617246280172463</v>
       </c>
       <c r="Q31">
-        <v>0.007633822384338224</v>
+        <v>0.007633755532337556</v>
       </c>
       <c r="R31">
-        <v>0.007633822384338224</v>
+        <v>0.007633755532337556</v>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -2004,7 +2004,7 @@
         <v>79</v>
       </c>
       <c r="C32">
-        <v>0.006351587919515879</v>
+        <v>0.006080640456806404</v>
       </c>
       <c r="D32">
         <v>-0.002000245952002459</v>
@@ -2013,31 +2013,31 @@
         <v>-0.007224030264240303</v>
       </c>
       <c r="G32">
-        <v>0.0008714469327144692</v>
+        <v>0.0008710422087104221</v>
       </c>
       <c r="I32">
         <v>0.000789382399893824</v>
       </c>
       <c r="J32">
-        <v>0.009773900391097082</v>
+        <v>0.008056055603086225</v>
       </c>
       <c r="K32">
-        <v>-0.0008645875526458756</v>
+        <v>-0.0008649681686496817</v>
       </c>
       <c r="L32">
-        <v>-0.0008645875526458756</v>
+        <v>-0.0008649681686496817</v>
       </c>
       <c r="O32">
-        <v>-0.0008645875526458756</v>
+        <v>-0.0008649681686496817</v>
       </c>
       <c r="P32">
-        <v>-0.0008698267766982677</v>
+        <v>-0.0008701761807017618</v>
       </c>
       <c r="Q32">
-        <v>-0.0008707431327074313</v>
+        <v>-0.0008705083767050838</v>
       </c>
       <c r="R32">
-        <v>-0.0008707431327074313</v>
+        <v>-0.0008705083767050838</v>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -2048,7 +2048,7 @@
         <v>80</v>
       </c>
       <c r="C33">
-        <v>0.009186885307868852</v>
+        <v>0.009066014466660144</v>
       </c>
       <c r="D33">
         <v>0.003653658888536589</v>
@@ -2057,31 +2057,31 @@
         <v>-0.01440284863202848</v>
       </c>
       <c r="G33">
-        <v>-0.006386005527860055</v>
+        <v>-0.006385750479857504</v>
       </c>
       <c r="I33">
         <v>-0.006636242874362428</v>
       </c>
       <c r="J33">
-        <v>-0.02559169451563344</v>
+        <v>-0.01216883257100708</v>
       </c>
       <c r="K33">
-        <v>0.006439775788397758</v>
+        <v>0.006439548508395485</v>
       </c>
       <c r="L33">
-        <v>0.006439775788397758</v>
+        <v>0.006439548508395485</v>
       </c>
       <c r="O33">
-        <v>0.006439775788397758</v>
+        <v>0.006439548508395485</v>
       </c>
       <c r="P33">
-        <v>0.006380212251802123</v>
+        <v>0.006380134647801347</v>
       </c>
       <c r="Q33">
-        <v>0.006427928824279288</v>
+        <v>0.006427958584279586</v>
       </c>
       <c r="R33">
-        <v>0.006427928824279288</v>
+        <v>0.006427958584279586</v>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -2092,7 +2092,7 @@
         <v>81</v>
       </c>
       <c r="C34">
-        <v>-0.01285640619256406</v>
+        <v>-0.0122299503862995</v>
       </c>
       <c r="D34">
         <v>-0.00284086194440862</v>
@@ -2101,31 +2101,31 @@
         <v>-0.001722985697229857</v>
       </c>
       <c r="G34">
-        <v>0.00149462396694624</v>
+        <v>0.001495053194950532</v>
       </c>
       <c r="I34">
         <v>0.001731148865311489</v>
       </c>
       <c r="J34">
-        <v>-0.001644224960729322</v>
+        <v>0.003332264789488134</v>
       </c>
       <c r="K34">
-        <v>-0.001464703286647033</v>
+        <v>-0.001463394422633944</v>
       </c>
       <c r="L34">
-        <v>-0.001464703286647033</v>
+        <v>-0.001463394422633944</v>
       </c>
       <c r="O34">
-        <v>-0.001464703286647033</v>
+        <v>-0.001463394422633944</v>
       </c>
       <c r="P34">
-        <v>-0.001487997074879971</v>
+        <v>-0.0014880699628807</v>
       </c>
       <c r="Q34">
-        <v>-0.001471527602715276</v>
+        <v>-0.001471327106713271</v>
       </c>
       <c r="R34">
-        <v>-0.001471527602715276</v>
+        <v>-0.001471327106713271</v>
       </c>
     </row>
     <row r="35" spans="1:18">
@@ -2136,7 +2136,7 @@
         <v>82</v>
       </c>
       <c r="C35">
-        <v>0.004804980216049803</v>
+        <v>0.00571469690114697</v>
       </c>
       <c r="D35">
         <v>0.006341509179415093</v>
@@ -2145,31 +2145,31 @@
         <v>0.02562687367626874</v>
       </c>
       <c r="G35">
-        <v>0.006941745381417453</v>
+        <v>0.006941301021413011</v>
       </c>
       <c r="I35">
         <v>0.007089926482899265</v>
       </c>
       <c r="J35">
-        <v>-0.006692276201637926</v>
+        <v>-0.002206691211302949</v>
       </c>
       <c r="K35">
-        <v>-0.007070437498704375</v>
+        <v>-0.007073944618739446</v>
       </c>
       <c r="L35">
-        <v>-0.007070437498704375</v>
+        <v>-0.007073944618739446</v>
       </c>
       <c r="O35">
-        <v>-0.007070437498704375</v>
+        <v>-0.007073944618739446</v>
       </c>
       <c r="P35">
-        <v>-0.006930149109301491</v>
+        <v>-0.006930032385300324</v>
       </c>
       <c r="Q35">
-        <v>-0.007022448730224487</v>
+        <v>-0.007022542258225422</v>
       </c>
       <c r="R35">
-        <v>-0.007022448730224487</v>
+        <v>-0.007022542258225422</v>
       </c>
     </row>
     <row r="36" spans="1:18">
@@ -2180,7 +2180,7 @@
         <v>83</v>
       </c>
       <c r="C36">
-        <v>0.003414187666141876</v>
+        <v>0.003641439168414392</v>
       </c>
       <c r="D36">
         <v>-0.00246730699267307</v>
@@ -2189,31 +2189,31 @@
         <v>-0.007362197197621972</v>
       </c>
       <c r="G36">
-        <v>-0.001408682642086826</v>
+        <v>-0.001408397858083978</v>
       </c>
       <c r="I36">
         <v>-0.00147308903073089</v>
       </c>
       <c r="J36">
-        <v>0.0002388994658442551</v>
+        <v>0.005974724762219042</v>
       </c>
       <c r="K36">
-        <v>0.001433910530339105</v>
+        <v>0.001438662746386627</v>
       </c>
       <c r="L36">
-        <v>0.001433910530339105</v>
+        <v>0.001438662746386627</v>
       </c>
       <c r="O36">
-        <v>0.001433910530339105</v>
+        <v>0.001438662746386627</v>
       </c>
       <c r="P36">
-        <v>0.001410656534106565</v>
+        <v>0.001410818894108189</v>
       </c>
       <c r="Q36">
-        <v>0.001422295298222953</v>
+        <v>0.001422742538227425</v>
       </c>
       <c r="R36">
-        <v>0.001422295298222953</v>
+        <v>0.001422742538227425</v>
       </c>
     </row>
     <row r="37" spans="1:18">
@@ -2224,7 +2224,7 @@
         <v>83</v>
       </c>
       <c r="C37">
-        <v>0.01123887820038878</v>
+        <v>0.01266725065867251</v>
       </c>
       <c r="D37">
         <v>-0.01519095769990958</v>
@@ -2233,31 +2233,31 @@
         <v>-0.007181248763812488</v>
       </c>
       <c r="G37">
-        <v>-0.008458122456581224</v>
+        <v>-0.008458565796585658</v>
       </c>
       <c r="I37">
         <v>-0.008833836568338365</v>
       </c>
       <c r="J37">
-        <v>-0.01247239028108002</v>
+        <v>-0.009047995112600469</v>
       </c>
       <c r="K37">
-        <v>0.008463386016633861</v>
+        <v>0.00846718492867185</v>
       </c>
       <c r="L37">
-        <v>0.008463386016633861</v>
+        <v>0.00846718492867185</v>
       </c>
       <c r="O37">
-        <v>0.008463386016633861</v>
+        <v>0.00846718492867185</v>
       </c>
       <c r="P37">
-        <v>0.008457592392575925</v>
+        <v>0.008457722136577223</v>
       </c>
       <c r="Q37">
-        <v>0.008461115748611157</v>
+        <v>0.008460940740609407</v>
       </c>
       <c r="R37">
-        <v>0.008461115748611157</v>
+        <v>0.008460940740609407</v>
       </c>
     </row>
     <row r="38" spans="1:18">
@@ -2268,7 +2268,7 @@
         <v>83</v>
       </c>
       <c r="C38">
-        <v>-0.02013763787737638</v>
+        <v>-0.01949335771493358</v>
       </c>
       <c r="D38">
         <v>-0.01165142259251423</v>
@@ -2277,31 +2277,31 @@
         <v>-0.001929280735292807</v>
       </c>
       <c r="G38">
-        <v>-0.001505735511057355</v>
+        <v>-0.001505894427058944</v>
       </c>
       <c r="I38">
         <v>-0.001471742186717422</v>
       </c>
       <c r="J38">
-        <v>0.01243108211993789</v>
+        <v>-0.004564813080218349</v>
       </c>
       <c r="K38">
-        <v>0.001539833559398335</v>
+        <v>0.001539550083395501</v>
       </c>
       <c r="L38">
-        <v>0.001539833559398335</v>
+        <v>0.001539550083395501</v>
       </c>
       <c r="O38">
-        <v>0.001539833559398335</v>
+        <v>0.001539550083395501</v>
       </c>
       <c r="P38">
-        <v>0.001506051423060514</v>
+        <v>0.001505677323056773</v>
       </c>
       <c r="Q38">
-        <v>0.001521189699211897</v>
+        <v>0.001521177303211773</v>
       </c>
       <c r="R38">
-        <v>0.001521189699211897</v>
+        <v>0.001521177303211773</v>
       </c>
     </row>
     <row r="39" spans="1:18">
@@ -2312,7 +2312,7 @@
         <v>83</v>
       </c>
       <c r="C39">
-        <v>0.01923086558430866</v>
+        <v>0.01975830402558304</v>
       </c>
       <c r="D39">
         <v>0.007499023610990236</v>
@@ -2321,31 +2321,31 @@
         <v>0.01510101622301016</v>
       </c>
       <c r="G39">
-        <v>0.01722613621626136</v>
+        <v>0.01722618421626184</v>
       </c>
       <c r="I39">
         <v>0.01703988767039888</v>
       </c>
       <c r="J39">
-        <v>0.003378617228449976</v>
+        <v>0.01488420707981582</v>
       </c>
       <c r="K39">
-        <v>-0.01725367282053673</v>
+        <v>-0.01725344812053448</v>
       </c>
       <c r="L39">
-        <v>-0.01725367282053673</v>
+        <v>-0.01725344812053448</v>
       </c>
       <c r="O39">
-        <v>-0.01725367282053673</v>
+        <v>-0.01725344812053448</v>
       </c>
       <c r="P39">
-        <v>-0.01722161123221611</v>
+        <v>-0.01722184648021846</v>
       </c>
       <c r="Q39">
-        <v>-0.01723929227239292</v>
+        <v>-0.01723906778839068</v>
       </c>
       <c r="R39">
-        <v>-0.01723929227239292</v>
+        <v>-0.01723906778839068</v>
       </c>
     </row>
     <row r="40" spans="1:18">
@@ -2356,7 +2356,7 @@
         <v>83</v>
       </c>
       <c r="C40">
-        <v>-0.00689788493697885</v>
+        <v>-0.007785020309850203</v>
       </c>
       <c r="D40">
         <v>-0.003414632878146329</v>
@@ -2365,31 +2365,31 @@
         <v>0.009693033564930335</v>
       </c>
       <c r="G40">
-        <v>0.0001215384372153844</v>
+        <v>0.0001213092492130925</v>
       </c>
       <c r="I40">
         <v>0.000224619506246195</v>
       </c>
       <c r="J40">
-        <v>-0.006372487607364858</v>
+        <v>0.009805627811054242</v>
       </c>
       <c r="K40">
-        <v>-0.0001675600456756005</v>
+        <v>-0.0001724163737241637</v>
       </c>
       <c r="L40">
-        <v>-0.0001675600456756005</v>
+        <v>-0.0001724163737241637</v>
       </c>
       <c r="O40">
-        <v>-0.0001675600456756005</v>
+        <v>-0.0001724163737241637</v>
       </c>
       <c r="P40">
-        <v>-0.0001104121811041218</v>
+        <v>-0.0001105711931057119</v>
       </c>
       <c r="Q40">
-        <v>-0.0001488815774888158</v>
+        <v>-0.0001497273134972731</v>
       </c>
       <c r="R40">
-        <v>-0.0001488815774888158</v>
+        <v>-0.0001497273134972731</v>
       </c>
     </row>
     <row r="41" spans="1:18">
@@ -2400,7 +2400,7 @@
         <v>84</v>
       </c>
       <c r="C41">
-        <v>-0.06774131699341317</v>
+        <v>-0.06239567150395671</v>
       </c>
       <c r="D41">
         <v>-0.0122099903780999</v>
@@ -2409,31 +2409,31 @@
         <v>-0.021411699970117</v>
       </c>
       <c r="G41">
-        <v>-0.02261586820615868</v>
+        <v>-0.02261542238215422</v>
       </c>
       <c r="I41">
         <v>-0.02288224132882241</v>
       </c>
       <c r="J41">
-        <v>-0.004866205771105237</v>
+        <v>-0.003792566591361009</v>
       </c>
       <c r="K41">
-        <v>0.02267222655472227</v>
+        <v>0.02267330498273305</v>
       </c>
       <c r="L41">
-        <v>0.02267222655472227</v>
+        <v>0.02267330498273305</v>
       </c>
       <c r="O41">
-        <v>0.02267222655472227</v>
+        <v>0.02267330498273305</v>
       </c>
       <c r="P41">
-        <v>0.02260719649007197</v>
+        <v>0.02260712492207125</v>
       </c>
       <c r="Q41">
-        <v>0.0226517202345172</v>
+        <v>0.02265177166651771</v>
       </c>
       <c r="R41">
-        <v>0.0226517202345172</v>
+        <v>0.02265177166651771</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final results for manuscript
</commit_message>
<xml_diff>
--- a/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
+++ b/biorefineries/oilcane/results/oilcane_spearman_-1.xlsx
@@ -794,40 +794,40 @@
         <v>55</v>
       </c>
       <c r="C4">
-        <v>0.0148164296321643</v>
+        <v>0.02026947980889813</v>
       </c>
       <c r="D4">
-        <v>0.00151221894312219</v>
+        <v>0.01112697495510899</v>
       </c>
       <c r="F4">
-        <v>0.01712925642329256</v>
+        <v>0.02372326248786348</v>
       </c>
       <c r="G4">
-        <v>0.0006357038103570381</v>
+        <v>0.009902970506296415</v>
       </c>
       <c r="I4">
-        <v>0.0006457376344573764</v>
+        <v>0.009801163160955676</v>
       </c>
       <c r="J4">
-        <v>0.001873686026875668</v>
+        <v>0.009107565618011697</v>
       </c>
       <c r="K4">
-        <v>-0.0007194071231940713</v>
+        <v>-0.01000318766411231</v>
       </c>
       <c r="L4">
-        <v>-0.0007194071231940713</v>
+        <v>-0.01000318766411231</v>
       </c>
       <c r="O4">
-        <v>-0.0007194071231940713</v>
+        <v>-0.01000318766411231</v>
       </c>
       <c r="P4">
-        <v>-0.0006269746742697467</v>
+        <v>-0.009891335170177113</v>
       </c>
       <c r="Q4">
-        <v>-0.0006918716829187168</v>
+        <v>-0.009968088085438878</v>
       </c>
       <c r="R4">
-        <v>-0.0006918716829187168</v>
+        <v>-0.009968088085438878</v>
       </c>
     </row>
     <row r="5" spans="1:31">
@@ -836,40 +836,40 @@
         <v>56</v>
       </c>
       <c r="C5">
-        <v>-0.005242748668427486</v>
+        <v>0.00771031359703615</v>
       </c>
       <c r="D5">
-        <v>0.0009778538137785381</v>
+        <v>-0.001765577465087148</v>
       </c>
       <c r="F5">
-        <v>-0.01525117390451174</v>
+        <v>0.0009094400532725009</v>
       </c>
       <c r="G5">
-        <v>-0.002193411789934117</v>
+        <v>-0.005989855781091498</v>
       </c>
       <c r="I5">
-        <v>-0.002392384391923844</v>
+        <v>-0.006081180235643442</v>
       </c>
       <c r="J5">
-        <v>-0.004755469532876422</v>
+        <v>-0.01403295255745915</v>
       </c>
       <c r="K5">
-        <v>0.002231237686312377</v>
+        <v>0.005995537124930268</v>
       </c>
       <c r="L5">
-        <v>0.002231237686312377</v>
+        <v>0.005995537124930268</v>
       </c>
       <c r="O5">
-        <v>0.002231237686312377</v>
+        <v>0.005995537124930268</v>
       </c>
       <c r="P5">
-        <v>0.002192748081927481</v>
+        <v>0.005991797343621834</v>
       </c>
       <c r="Q5">
-        <v>0.002206465930064659</v>
+        <v>0.005992438757694357</v>
       </c>
       <c r="R5">
-        <v>0.002206465930064659</v>
+        <v>0.005992438757694357</v>
       </c>
     </row>
     <row r="6" spans="1:31">
@@ -878,40 +878,40 @@
         <v>57</v>
       </c>
       <c r="C6">
-        <v>0.2828656471286564</v>
+        <v>0.2744483080304423</v>
       </c>
       <c r="D6">
-        <v>-0.02621256331012563</v>
+        <v>-0.01058144402471006</v>
       </c>
       <c r="F6">
-        <v>-0.492902494845025</v>
+        <v>-0.4974943736405372</v>
       </c>
       <c r="G6">
-        <v>-0.6208497665684977</v>
+        <v>-0.6102427030975424</v>
       </c>
       <c r="I6">
-        <v>-0.6213371147013711</v>
+        <v>-0.6103569726540152</v>
       </c>
       <c r="J6">
-        <v>-0.000700843192824616</v>
+        <v>-0.005299507990749185</v>
       </c>
       <c r="K6">
-        <v>0.6208431347804313</v>
+        <v>0.6102921337467522</v>
       </c>
       <c r="L6">
-        <v>0.6208431347804313</v>
+        <v>0.6102921337467522</v>
       </c>
       <c r="O6">
-        <v>0.6208431347804313</v>
+        <v>0.6102921337467522</v>
       </c>
       <c r="P6">
-        <v>0.620852303200523</v>
+        <v>0.6102401357068772</v>
       </c>
       <c r="Q6">
-        <v>0.6208391764843918</v>
+        <v>0.6102830509419227</v>
       </c>
       <c r="R6">
-        <v>0.6208391764843918</v>
+        <v>0.6102830509419227</v>
       </c>
     </row>
     <row r="7" spans="1:31">
@@ -920,40 +920,40 @@
         <v>58</v>
       </c>
       <c r="C7">
-        <v>0.01030776876707769</v>
+        <v>-0.01354387511787305</v>
       </c>
       <c r="D7">
-        <v>0.02194901197549012</v>
+        <v>-0.00489838524059977</v>
       </c>
       <c r="F7">
-        <v>0.02374809681348097</v>
+        <v>0.0004242228113159815</v>
       </c>
       <c r="G7">
-        <v>0.02247264428072644</v>
+        <v>0.01219808294840755</v>
       </c>
       <c r="I7">
-        <v>0.02254483872944839</v>
+        <v>0.01230879005169985</v>
       </c>
       <c r="J7">
-        <v>0.009543290109709992</v>
+        <v>-0.007838194380120391</v>
       </c>
       <c r="K7">
-        <v>-0.02250033418500334</v>
+        <v>-0.01217461373710334</v>
       </c>
       <c r="L7">
-        <v>-0.02250033418500334</v>
+        <v>-0.01217461373710334</v>
       </c>
       <c r="O7">
-        <v>-0.02250033418500334</v>
+        <v>-0.01217461373710334</v>
       </c>
       <c r="P7">
-        <v>-0.02247407370874074</v>
+        <v>-0.01220434762819293</v>
       </c>
       <c r="Q7">
-        <v>-0.02248712856887129</v>
+        <v>-0.01217914024498657</v>
       </c>
       <c r="R7">
-        <v>-0.02248712856887129</v>
+        <v>-0.01217914024498657</v>
       </c>
     </row>
     <row r="8" spans="1:31">
@@ -962,40 +962,40 @@
         <v>59</v>
       </c>
       <c r="C8">
-        <v>0.2684335947083359</v>
+        <v>0.2926001708687527</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="F8">
-        <v>0.6224610370166104</v>
+        <v>0.6099145184439769</v>
       </c>
       <c r="G8">
-        <v>0.7875797851957979</v>
+        <v>0.7852589787774842</v>
       </c>
       <c r="I8">
-        <v>0.787382098681821</v>
+        <v>0.7853885075763831</v>
       </c>
       <c r="J8">
-        <v>-6.668716596108231E-05</v>
+        <v>-0.01485399726394193</v>
       </c>
       <c r="K8">
-        <v>-0.7875819821558198</v>
+        <v>-0.7852174441049602</v>
       </c>
       <c r="L8">
-        <v>-0.7875819821558198</v>
+        <v>-0.7852174441049602</v>
       </c>
       <c r="O8">
-        <v>-0.7875819821558198</v>
+        <v>-0.7852174441049602</v>
       </c>
       <c r="P8">
-        <v>-0.787576802535768</v>
+        <v>-0.7852601092384394</v>
       </c>
       <c r="Q8">
-        <v>-0.7875889731038898</v>
+        <v>-0.7852259420972805</v>
       </c>
       <c r="R8">
-        <v>-0.7875889731038898</v>
+        <v>-0.7852259420972805</v>
       </c>
     </row>
     <row r="9" spans="1:31">
@@ -1006,40 +1006,40 @@
         <v>60</v>
       </c>
       <c r="C9">
-        <v>-0.004327833211278332</v>
+        <v>0.004393171240518301</v>
       </c>
       <c r="D9">
-        <v>-0.009849915098499151</v>
+        <v>0.01311056793141513</v>
       </c>
       <c r="F9">
-        <v>-0.005273047624730476</v>
+        <v>0.01118234126847409</v>
       </c>
       <c r="G9">
-        <v>-0.0008179209441792094</v>
+        <v>0.006980964530952572</v>
       </c>
       <c r="I9">
-        <v>-0.0003577986275779863</v>
+        <v>0.007469362827646295</v>
       </c>
       <c r="J9">
-        <v>-0.004876688950829339</v>
+        <v>-0.004910901073558926</v>
       </c>
       <c r="K9">
-        <v>0.0008287248802872489</v>
+        <v>-0.007034782844293483</v>
       </c>
       <c r="L9">
-        <v>0.0008287248802872489</v>
+        <v>-0.007034782844293483</v>
       </c>
       <c r="O9">
-        <v>0.0008287248802872489</v>
+        <v>-0.007034782844293483</v>
       </c>
       <c r="P9">
-        <v>0.0008103354921033551</v>
+        <v>-0.006978778538730915</v>
       </c>
       <c r="Q9">
-        <v>0.0008343521123435211</v>
+        <v>-0.007012116883001828</v>
       </c>
       <c r="R9">
-        <v>0.0008343521123435211</v>
+        <v>-0.007012116883001828</v>
       </c>
     </row>
     <row r="10" spans="1:31">
@@ -1050,40 +1050,40 @@
         <v>60</v>
       </c>
       <c r="C10">
-        <v>0.8240005612520057</v>
+        <v>0.8189702157417222</v>
       </c>
       <c r="D10">
-        <v>-0.006061106124611061</v>
+        <v>0.01630515048914298</v>
       </c>
       <c r="F10">
-        <v>-0.009698970816989708</v>
+        <v>0.02227498105898408</v>
       </c>
       <c r="G10">
-        <v>-0.01136968310969683</v>
+        <v>0.0248626941931671</v>
       </c>
       <c r="I10">
-        <v>-0.01126867538868675</v>
+        <v>0.02479791802809247</v>
       </c>
       <c r="J10">
-        <v>-0.01583476228550769</v>
+        <v>-0.01487121437314347</v>
       </c>
       <c r="K10">
-        <v>0.01138975754989758</v>
+        <v>-0.02485063899766624</v>
       </c>
       <c r="L10">
-        <v>0.01138975754989758</v>
+        <v>-0.02485063899766624</v>
       </c>
       <c r="O10">
-        <v>0.01138975754989758</v>
+        <v>-0.02485063899766624</v>
       </c>
       <c r="P10">
-        <v>0.01137315092973151</v>
+        <v>-0.02486373031818329</v>
       </c>
       <c r="Q10">
-        <v>0.0113882702578827</v>
+        <v>-0.02485898002904657</v>
       </c>
       <c r="R10">
-        <v>0.0113882702578827</v>
+        <v>-0.02485898002904657</v>
       </c>
     </row>
     <row r="11" spans="1:31">
@@ -1094,40 +1094,40 @@
         <v>60</v>
       </c>
       <c r="C11">
-        <v>0.001205539308055393</v>
+        <v>-0.002378024662156635</v>
       </c>
       <c r="D11">
-        <v>-1.081171210811712E-05</v>
+        <v>-0.002207518206367472</v>
       </c>
       <c r="F11">
-        <v>0.01481179351611794</v>
+        <v>-0.00396997817921841</v>
       </c>
       <c r="G11">
-        <v>0.00468864202688642</v>
+        <v>-0.004738018808406544</v>
       </c>
       <c r="I11">
-        <v>0.004428350672283508</v>
+        <v>-0.00481345786427278</v>
       </c>
       <c r="J11">
-        <v>-0.01407036079278574</v>
+        <v>0.009116543675567209</v>
       </c>
       <c r="K11">
-        <v>-0.004781005403810054</v>
+        <v>0.004759118863423732</v>
       </c>
       <c r="L11">
-        <v>-0.004781005403810054</v>
+        <v>0.004759118863423732</v>
       </c>
       <c r="O11">
-        <v>-0.004781005403810054</v>
+        <v>0.004759118863423732</v>
       </c>
       <c r="P11">
-        <v>-0.004677374842773749</v>
+        <v>0.004734694691167106</v>
       </c>
       <c r="Q11">
-        <v>-0.004738099379380994</v>
+        <v>0.004747992097624877</v>
       </c>
       <c r="R11">
-        <v>-0.004738099379380994</v>
+        <v>0.004747992097624877</v>
       </c>
     </row>
     <row r="12" spans="1:31">
@@ -1138,40 +1138,40 @@
         <v>61</v>
       </c>
       <c r="C12">
-        <v>0.02266218575862185</v>
+        <v>-0.0006586848852919514</v>
       </c>
       <c r="D12">
-        <v>0.01840892352408923</v>
+        <v>0.005172416705819012</v>
       </c>
       <c r="F12">
-        <v>0.006248929538489295</v>
+        <v>0.01160835273606801</v>
       </c>
       <c r="G12">
-        <v>0.01013836278538363</v>
+        <v>-0.002120775056574611</v>
       </c>
       <c r="I12">
-        <v>0.01012691094526911</v>
+        <v>-0.001946439522600618</v>
       </c>
       <c r="J12">
-        <v>0.0004537099816154965</v>
+        <v>-0.01335879006974242</v>
       </c>
       <c r="K12">
-        <v>-0.01014380634543806</v>
+        <v>0.002021550992524235</v>
       </c>
       <c r="L12">
-        <v>-0.01014380634543806</v>
+        <v>0.002021550992524235</v>
       </c>
       <c r="O12">
-        <v>-0.01014380634543806</v>
+        <v>0.002021550992524235</v>
       </c>
       <c r="P12">
-        <v>-0.01013550437335504</v>
+        <v>0.002132366775505731</v>
       </c>
       <c r="Q12">
-        <v>-0.01013627480936275</v>
+        <v>0.002056657368072772</v>
       </c>
       <c r="R12">
-        <v>-0.01013627480936275</v>
+        <v>0.002056657368072772</v>
       </c>
     </row>
     <row r="13" spans="1:31">
@@ -1182,40 +1182,40 @@
         <v>62</v>
       </c>
       <c r="C13">
-        <v>0.05010769224907692</v>
+        <v>0.05692399849099998</v>
       </c>
       <c r="D13">
-        <v>-0.02004360854043609</v>
+        <v>-0.01257064383704131</v>
       </c>
       <c r="F13">
-        <v>-0.007983215575832156</v>
+        <v>-0.008784274402879289</v>
       </c>
       <c r="G13">
-        <v>-0.008683869242838692</v>
+        <v>-0.01242641161603768</v>
       </c>
       <c r="I13">
-        <v>-0.008591242561912425</v>
+        <v>-0.01234527560695743</v>
       </c>
       <c r="J13">
-        <v>0.009259240951473371</v>
+        <v>-0.005740004695481516</v>
       </c>
       <c r="K13">
-        <v>0.008689972202899724</v>
+        <v>0.01243721527245649</v>
       </c>
       <c r="L13">
-        <v>0.008689972202899724</v>
+        <v>0.01243721527245649</v>
       </c>
       <c r="O13">
-        <v>0.008689972202899724</v>
+        <v>0.01243721527245649</v>
       </c>
       <c r="P13">
-        <v>0.0086772297987723</v>
+        <v>0.01242969764733903</v>
       </c>
       <c r="Q13">
-        <v>0.008689141202891413</v>
+        <v>0.01243127403017616</v>
       </c>
       <c r="R13">
-        <v>0.008689141202891413</v>
+        <v>0.01243127403017616</v>
       </c>
     </row>
     <row r="14" spans="1:31">
@@ -1224,40 +1224,40 @@
         <v>63</v>
       </c>
       <c r="C14">
-        <v>-0.3542953498709535</v>
+        <v>-0.3635505653757902</v>
       </c>
       <c r="D14">
-        <v>-0.003031562910315629</v>
+        <v>-0.007575327587114496</v>
       </c>
       <c r="F14">
-        <v>-0.0125199202251992</v>
+        <v>0.008219756237808693</v>
       </c>
       <c r="G14">
-        <v>-0.01390005859900059</v>
+        <v>-0.00256524922758202</v>
       </c>
       <c r="I14">
-        <v>-0.01418066613380666</v>
+        <v>-0.002563699704120308</v>
       </c>
       <c r="J14">
-        <v>0.001565608492603544</v>
+        <v>-0.006118645171148682</v>
       </c>
       <c r="K14">
-        <v>0.01392549905525499</v>
+        <v>0.002427413803553341</v>
       </c>
       <c r="L14">
-        <v>0.01392549905525499</v>
+        <v>0.002427413803553341</v>
       </c>
       <c r="O14">
-        <v>0.01392549905525499</v>
+        <v>0.002427413803553341</v>
       </c>
       <c r="P14">
-        <v>0.01389444315094443</v>
+        <v>0.00257504830586013</v>
       </c>
       <c r="Q14">
-        <v>0.01391916102719161</v>
+        <v>0.002482229804409841</v>
       </c>
       <c r="R14">
-        <v>0.01391916102719161</v>
+        <v>0.002482229804409841</v>
       </c>
     </row>
     <row r="15" spans="1:31">
@@ -1268,40 +1268,40 @@
         <v>64</v>
       </c>
       <c r="C15">
-        <v>0.00107900095079001</v>
+        <v>-0.01771713988620531</v>
       </c>
       <c r="D15">
-        <v>-0.002824025776240258</v>
+        <v>-0.01679604588743822</v>
       </c>
       <c r="F15">
-        <v>-0.004522843185228432</v>
+        <v>-0.01991605156118831</v>
       </c>
       <c r="G15">
-        <v>-0.006673683882736838</v>
+        <v>-0.01796145154627269</v>
       </c>
       <c r="I15">
-        <v>-0.006586563185865632</v>
+        <v>-0.0180370237505785</v>
       </c>
       <c r="J15">
-        <v>0.01015344027457751</v>
+        <v>-0.01399927969259424</v>
       </c>
       <c r="K15">
-        <v>0.006667343538673435</v>
+        <v>0.01799946721874168</v>
       </c>
       <c r="L15">
-        <v>0.006667343538673435</v>
+        <v>0.01799946721874168</v>
       </c>
       <c r="O15">
-        <v>0.006667343538673435</v>
+        <v>0.01799946721874168</v>
       </c>
       <c r="P15">
-        <v>0.006675547566755476</v>
+        <v>0.01795571606180807</v>
       </c>
       <c r="Q15">
-        <v>0.006663872346638724</v>
+        <v>0.01799428713272324</v>
       </c>
       <c r="R15">
-        <v>0.006663872346638724</v>
+        <v>0.01799428713272324</v>
       </c>
     </row>
     <row r="16" spans="1:31">
@@ -1312,40 +1312,40 @@
         <v>64</v>
       </c>
       <c r="C16">
-        <v>-0.007867395522673955</v>
+        <v>0.02341835422528679</v>
       </c>
       <c r="D16">
-        <v>0.0007758225677582258</v>
+        <v>0.008682973330983959</v>
       </c>
       <c r="F16">
-        <v>-0.002102966469029665</v>
+        <v>-0.01332128066908251</v>
       </c>
       <c r="G16">
-        <v>-0.001063054462630545</v>
+        <v>-0.006897270271832349</v>
       </c>
       <c r="I16">
-        <v>-0.0008461253484612535</v>
+        <v>-0.006648696174198379</v>
       </c>
       <c r="J16">
-        <v>-0.008438939242291991</v>
+        <v>0.01433824433144368</v>
       </c>
       <c r="K16">
-        <v>0.001033075906330759</v>
+        <v>0.006961317765020591</v>
       </c>
       <c r="L16">
-        <v>0.001033075906330759</v>
+        <v>0.006961317765020591</v>
       </c>
       <c r="O16">
-        <v>0.001033075906330759</v>
+        <v>0.006961317765020591</v>
       </c>
       <c r="P16">
-        <v>0.001065458734654587</v>
+        <v>0.006891090388923288</v>
       </c>
       <c r="Q16">
-        <v>0.001046190742461908</v>
+        <v>0.006930547420789804</v>
       </c>
       <c r="R16">
-        <v>0.001046190742461908</v>
+        <v>0.006930547420789804</v>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -1356,40 +1356,40 @@
         <v>65</v>
       </c>
       <c r="C17">
-        <v>0.01014700625347006</v>
+        <v>0.01277119667611245</v>
       </c>
       <c r="D17">
-        <v>0.01176501519365015</v>
+        <v>0.01099503082804736</v>
       </c>
       <c r="F17">
-        <v>-0.002081501528815015</v>
+        <v>0.007119458079991535</v>
       </c>
       <c r="G17">
-        <v>-0.004309450759094508</v>
+        <v>0.001386322310723786</v>
       </c>
       <c r="I17">
-        <v>-0.004342034131420341</v>
+        <v>0.001224969722265152</v>
       </c>
       <c r="J17">
-        <v>0.007058441736929497</v>
+        <v>0.005235253431558368</v>
       </c>
       <c r="K17">
-        <v>0.004306603375066035</v>
+        <v>-0.001414142647095979</v>
       </c>
       <c r="L17">
-        <v>0.004306603375066035</v>
+        <v>-0.001414142647095979</v>
       </c>
       <c r="O17">
-        <v>0.004306603375066035</v>
+        <v>-0.001414142647095979</v>
       </c>
       <c r="P17">
-        <v>0.004311253795112538</v>
+        <v>-0.001374740224605316</v>
       </c>
       <c r="Q17">
-        <v>0.004312354567123546</v>
+        <v>-0.001408114662626792</v>
       </c>
       <c r="R17">
-        <v>0.004312354567123546</v>
+        <v>-0.001408114662626792</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -1400,40 +1400,40 @@
         <v>64</v>
       </c>
       <c r="C18">
-        <v>0.009169314655693147</v>
+        <v>0.0070132287111442</v>
       </c>
       <c r="D18">
-        <v>-0.001414514918145149</v>
+        <v>0.002837576856837139</v>
       </c>
       <c r="F18">
-        <v>-0.001909786711097867</v>
+        <v>0.003178427276225426</v>
       </c>
       <c r="G18">
-        <v>-0.00581824093018241</v>
+        <v>0.00821634228463035</v>
       </c>
       <c r="I18">
-        <v>-0.005864057662640577</v>
+        <v>0.008238016534969009</v>
       </c>
       <c r="J18">
-        <v>-0.01738753261916367</v>
+        <v>0.00910492694859997</v>
       </c>
       <c r="K18">
-        <v>0.005802721726027218</v>
+        <v>-0.008187617471681523</v>
       </c>
       <c r="L18">
-        <v>0.005802721726027218</v>
+        <v>-0.008187617471681523</v>
       </c>
       <c r="O18">
-        <v>0.005802721726027218</v>
+        <v>-0.008187617471681523</v>
       </c>
       <c r="P18">
-        <v>0.005820913306209132</v>
+        <v>-0.008218147534658557</v>
       </c>
       <c r="Q18">
-        <v>0.005822729290227292</v>
+        <v>-0.008202625885978532</v>
       </c>
       <c r="R18">
-        <v>0.005822729290227292</v>
+        <v>-0.008202625885978532</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -1442,40 +1442,40 @@
         <v>66</v>
       </c>
       <c r="C19">
-        <v>0.01459265887392659</v>
+        <v>-0.009654243221160052</v>
       </c>
       <c r="D19">
-        <v>0.01707790277077903</v>
+        <v>-0.02570739963605312</v>
       </c>
       <c r="F19">
-        <v>0.00673844303538443</v>
+        <v>-0.03856192799315513</v>
       </c>
       <c r="G19">
-        <v>0.002646988082469881</v>
+        <v>-0.02990476230319941</v>
       </c>
       <c r="I19">
-        <v>0.0026238800422388</v>
+        <v>-0.03026305500411024</v>
       </c>
       <c r="J19">
-        <v>0.01521541544582149</v>
+        <v>-0.0006088189418750908</v>
       </c>
       <c r="K19">
-        <v>-0.002631095714310957</v>
+        <v>0.03001181266424708</v>
       </c>
       <c r="L19">
-        <v>-0.002631095714310957</v>
+        <v>0.03001181266424708</v>
       </c>
       <c r="O19">
-        <v>-0.002631095714310957</v>
+        <v>0.03001181266424708</v>
       </c>
       <c r="P19">
-        <v>-0.002652283466522835</v>
+        <v>0.02989769001402641</v>
       </c>
       <c r="Q19">
-        <v>-0.002632375826323758</v>
+        <v>0.02997610589025166</v>
       </c>
       <c r="R19">
-        <v>-0.002632375826323758</v>
+        <v>0.02997610589025166</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -1486,40 +1486,40 @@
         <v>67</v>
       </c>
       <c r="C20">
-        <v>-0.006772085455720854</v>
+        <v>-0.007311842059560034</v>
       </c>
       <c r="D20">
-        <v>-0.007641676312416763</v>
+        <v>0.006780813410637711</v>
       </c>
       <c r="F20">
-        <v>-0.01275603319956033</v>
+        <v>0.004988586406071663</v>
       </c>
       <c r="G20">
-        <v>-0.01273863918738639</v>
+        <v>-0.003072387868318561</v>
       </c>
       <c r="I20">
-        <v>-0.01277064880370649</v>
+        <v>-0.00303517757867465</v>
       </c>
       <c r="J20">
-        <v>-0.0246030375246055</v>
+        <v>0.007063877900460101</v>
       </c>
       <c r="K20">
-        <v>0.01279567872795679</v>
+        <v>0.003061016719703387</v>
       </c>
       <c r="L20">
-        <v>0.01279567872795679</v>
+        <v>0.003061016719703387</v>
       </c>
       <c r="O20">
-        <v>0.01279567872795679</v>
+        <v>0.003061016719703387</v>
       </c>
       <c r="P20">
-        <v>0.01273885110738851</v>
+        <v>0.003081099352829678</v>
       </c>
       <c r="Q20">
-        <v>0.01276613907166139</v>
+        <v>0.003060499969695313</v>
       </c>
       <c r="R20">
-        <v>0.01276613907166139</v>
+        <v>0.003060499969695313</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -1530,40 +1530,40 @@
         <v>68</v>
       </c>
       <c r="C21">
-        <v>-0.001864848102648481</v>
+        <v>0.01148690127323283</v>
       </c>
       <c r="D21">
-        <v>0.004832216064322161</v>
+        <v>-0.0001334091348970178</v>
       </c>
       <c r="F21">
-        <v>0.008761591539615915</v>
+        <v>-0.00554296377410881</v>
       </c>
       <c r="G21">
-        <v>0.01026772164667722</v>
+        <v>-0.01030248510628883</v>
       </c>
       <c r="I21">
-        <v>0.01016340810563408</v>
+        <v>-0.0102350459958601</v>
       </c>
       <c r="J21">
-        <v>0.004325829066586761</v>
+        <v>-0.005665142044231468</v>
       </c>
       <c r="K21">
-        <v>-0.01026386850663868</v>
+        <v>0.01029869179372956</v>
       </c>
       <c r="L21">
-        <v>-0.01026386850663868</v>
+        <v>0.01029869179372956</v>
       </c>
       <c r="O21">
-        <v>-0.01026386850663868</v>
+        <v>0.01029869179372956</v>
       </c>
       <c r="P21">
-        <v>-0.01027046449870465</v>
+        <v>0.01030573818446466</v>
       </c>
       <c r="Q21">
-        <v>-0.01026454063864541</v>
+        <v>0.01030061146563456</v>
       </c>
       <c r="R21">
-        <v>-0.01026454063864541</v>
+        <v>0.01030061146563456</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -1572,40 +1572,40 @@
         <v>69</v>
       </c>
       <c r="C22">
-        <v>-0.01586492279064923</v>
+        <v>-0.01561019693922183</v>
       </c>
       <c r="D22">
-        <v>-7.972794079727941E-05</v>
+        <v>0.0117859004966547</v>
       </c>
       <c r="F22">
-        <v>0.02701235296212353</v>
+        <v>0.005151178627362167</v>
       </c>
       <c r="G22">
-        <v>0.01163395396433954</v>
+        <v>0.003376835396513053</v>
       </c>
       <c r="I22">
-        <v>0.01163227119232271</v>
+        <v>0.003550053922657093</v>
       </c>
       <c r="J22">
-        <v>0.008407619532811611</v>
+        <v>-0.004709614128016769</v>
       </c>
       <c r="K22">
-        <v>-0.01175150354151503</v>
+        <v>-0.00338787961543562</v>
       </c>
       <c r="L22">
-        <v>-0.01175150354151503</v>
+        <v>-0.00338787961543562</v>
       </c>
       <c r="O22">
-        <v>-0.01175150354151503</v>
+        <v>-0.00338787961543562</v>
       </c>
       <c r="P22">
-        <v>-0.01162198329221983</v>
+        <v>-0.003381519873148749</v>
       </c>
       <c r="Q22">
-        <v>-0.01170356445303565</v>
+        <v>-0.00338909177951706</v>
       </c>
       <c r="R22">
-        <v>-0.01170356445303565</v>
+        <v>-0.00338909177951706</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -1614,40 +1614,40 @@
         <v>70</v>
       </c>
       <c r="C23">
-        <v>0.01001863292818633</v>
+        <v>-0.005139266166238535</v>
       </c>
       <c r="D23">
-        <v>0.01001911825619118</v>
+        <v>-0.02077025807453528</v>
       </c>
       <c r="F23">
-        <v>0.007504299915042999</v>
+        <v>-0.02586758278699349</v>
       </c>
       <c r="G23">
-        <v>-0.002179117089791171</v>
+        <v>-0.02001940571124072</v>
       </c>
       <c r="I23">
-        <v>-0.002599315189993152</v>
+        <v>-0.02022986937859171</v>
       </c>
       <c r="J23">
-        <v>-0.008192914276423557</v>
+        <v>0.006895584940245109</v>
       </c>
       <c r="K23">
-        <v>0.002088460628884606</v>
+        <v>0.02010989281421708</v>
       </c>
       <c r="L23">
-        <v>0.002088460628884606</v>
+        <v>0.02010989281421708</v>
       </c>
       <c r="O23">
-        <v>0.002088460628884606</v>
+        <v>0.02010989281421708</v>
       </c>
       <c r="P23">
-        <v>0.00217650399376504</v>
+        <v>0.02000054550782103</v>
       </c>
       <c r="Q23">
-        <v>0.002123430189234302</v>
+        <v>0.0200618620400291</v>
       </c>
       <c r="R23">
-        <v>0.002123430189234302</v>
+        <v>0.0200618620400291</v>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -1656,40 +1656,40 @@
         <v>71</v>
       </c>
       <c r="C24">
-        <v>-0.00610967290909673</v>
+        <v>0.000800923442201929</v>
       </c>
       <c r="D24">
-        <v>-0.01110188474701885</v>
+        <v>0.001018814640918979</v>
       </c>
       <c r="F24">
-        <v>-0.0153320895453209</v>
+        <v>0.01214169183033894</v>
       </c>
       <c r="G24">
-        <v>-0.01419712702597127</v>
+        <v>0.006775062012110345</v>
       </c>
       <c r="I24">
-        <v>-0.01401925282419253</v>
+        <v>0.006910915303295552</v>
       </c>
       <c r="J24">
-        <v>0.005401212400257207</v>
+        <v>-0.0201762481730616</v>
       </c>
       <c r="K24">
-        <v>0.0142294406382944</v>
+        <v>-0.006837299544332807</v>
       </c>
       <c r="L24">
-        <v>0.0142294406382944</v>
+        <v>-0.006837299544332807</v>
       </c>
       <c r="O24">
-        <v>0.0142294406382944</v>
+        <v>-0.006837299544332807</v>
       </c>
       <c r="P24">
-        <v>0.01419045251790452</v>
+        <v>-0.006770527629226995</v>
       </c>
       <c r="Q24">
-        <v>0.01421851195018512</v>
+        <v>-0.006814301520535962</v>
       </c>
       <c r="R24">
-        <v>0.01421851195018512</v>
+        <v>-0.006814301520535962</v>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -1700,40 +1700,40 @@
         <v>72</v>
       </c>
       <c r="C25">
-        <v>-0.001126837331268374</v>
+        <v>-0.02295415360084615</v>
       </c>
       <c r="D25">
-        <v>0.001704990857049909</v>
+        <v>-0.01706367614943245</v>
       </c>
       <c r="F25">
-        <v>-0.001873821138738211</v>
+        <v>-0.006547959922624374</v>
       </c>
       <c r="G25">
-        <v>-0.00262980297829803</v>
+        <v>-0.006124079744126247</v>
       </c>
       <c r="I25">
-        <v>-0.00269752502697525</v>
+        <v>-0.006026652281666443</v>
       </c>
       <c r="J25">
-        <v>0.009899400990695362</v>
+        <v>0.02047705663941474</v>
       </c>
       <c r="K25">
-        <v>0.002623444886234449</v>
+        <v>0.006146749314792959</v>
       </c>
       <c r="L25">
-        <v>0.002623444886234449</v>
+        <v>0.006146749314792959</v>
       </c>
       <c r="O25">
-        <v>0.002623444886234449</v>
+        <v>0.006146749314792959</v>
       </c>
       <c r="P25">
-        <v>0.002633286158332862</v>
+        <v>0.006117662509650977</v>
       </c>
       <c r="Q25">
-        <v>0.002630777474307775</v>
+        <v>0.006129736830152139</v>
       </c>
       <c r="R25">
-        <v>0.002630777474307775</v>
+        <v>0.006129736830152139</v>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -1742,40 +1742,40 @@
         <v>73</v>
       </c>
       <c r="C26">
-        <v>0.01545045230250452</v>
+        <v>-0.01932006904406358</v>
       </c>
       <c r="D26">
-        <v>-0.01081725564017256</v>
+        <v>0.007981843437216304</v>
       </c>
       <c r="F26">
-        <v>-0.02193400050334001</v>
+        <v>0.01565463158054112</v>
       </c>
       <c r="G26">
-        <v>-0.01488172783681728</v>
+        <v>0.01275920450405007</v>
       </c>
       <c r="I26">
-        <v>-0.0150762303067623</v>
+        <v>0.01288752842793013</v>
       </c>
       <c r="J26">
-        <v>-0.02005703061303707</v>
+        <v>-0.0003673214656505533</v>
       </c>
       <c r="K26">
-        <v>0.01495130618951306</v>
+        <v>-0.01276687897291999</v>
       </c>
       <c r="L26">
-        <v>0.01495130618951306</v>
+        <v>-0.01276687897291999</v>
       </c>
       <c r="O26">
-        <v>0.01495130618951306</v>
+        <v>-0.01276687897291999</v>
       </c>
       <c r="P26">
-        <v>0.0148752400727524</v>
+        <v>-0.01275738048058407</v>
       </c>
       <c r="Q26">
-        <v>0.01491661050516611</v>
+        <v>-0.01276579519946555</v>
       </c>
       <c r="R26">
-        <v>0.01491661050516611</v>
+        <v>-0.01276579519946555</v>
       </c>
     </row>
     <row r="27" spans="1:18">
@@ -1786,40 +1786,40 @@
         <v>74</v>
       </c>
       <c r="C27">
-        <v>0.003098167050981671</v>
+        <v>0.003599051610922682</v>
       </c>
       <c r="D27">
-        <v>-0.001261675212616752</v>
+        <v>0.02903286291457599</v>
       </c>
       <c r="F27">
-        <v>-0.006484291600842916</v>
+        <v>-0.004948963741390059</v>
       </c>
       <c r="G27">
-        <v>-0.00272717699127177</v>
+        <v>0.004623137064424017</v>
       </c>
       <c r="I27">
-        <v>-0.002869706212697062</v>
+        <v>0.004870385302662271</v>
       </c>
       <c r="J27">
-        <v>-0.01790454949168588</v>
+        <v>0.004206499342078385</v>
       </c>
       <c r="K27">
-        <v>0.002768992671689926</v>
+        <v>-0.004588638798259982</v>
       </c>
       <c r="L27">
-        <v>0.002768992671689926</v>
+        <v>-0.004588638798259982</v>
       </c>
       <c r="O27">
-        <v>0.002768992671689926</v>
+        <v>-0.004588638798259982</v>
       </c>
       <c r="P27">
-        <v>0.002723668899236689</v>
+        <v>-0.00462524993164453</v>
       </c>
       <c r="Q27">
-        <v>0.002742690819426909</v>
+        <v>-0.004601929735967653</v>
       </c>
       <c r="R27">
-        <v>0.002742690819426909</v>
+        <v>-0.004601929735967653</v>
       </c>
     </row>
     <row r="28" spans="1:18">
@@ -1828,40 +1828,40 @@
         <v>75</v>
       </c>
       <c r="C28">
-        <v>-0.0009040174890401748</v>
+        <v>-0.009338444958413204</v>
       </c>
       <c r="D28">
-        <v>0.01474209685542097</v>
+        <v>0.009685264065394753</v>
       </c>
       <c r="F28">
-        <v>-0.0002166517941665179</v>
+        <v>0.01562017407219022</v>
       </c>
       <c r="G28">
-        <v>0.003176748415767484</v>
+        <v>0.004345110677267355</v>
       </c>
       <c r="I28">
-        <v>0.003240781484407815</v>
+        <v>0.004180021026250329</v>
       </c>
       <c r="J28">
-        <v>-0.0007549402438115624</v>
+        <v>-0.01046326949151028</v>
       </c>
       <c r="K28">
-        <v>-0.003162592063625921</v>
+        <v>-0.004407190662612354</v>
       </c>
       <c r="L28">
-        <v>-0.003162592063625921</v>
+        <v>-0.004407190662612354</v>
       </c>
       <c r="O28">
-        <v>-0.003162592063625921</v>
+        <v>-0.004407190662612354</v>
       </c>
       <c r="P28">
-        <v>-0.003170627707706277</v>
+        <v>-0.004336414474006477</v>
       </c>
       <c r="Q28">
-        <v>-0.003172870267728703</v>
+        <v>-0.004384575045071486</v>
       </c>
       <c r="R28">
-        <v>-0.003172870267728703</v>
+        <v>-0.004384575045071486</v>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -1872,40 +1872,40 @@
         <v>76</v>
       </c>
       <c r="C29">
-        <v>0.006421504540215046</v>
+        <v>-0.01206652469635195</v>
       </c>
       <c r="D29">
-        <v>-0.005577593131775931</v>
+        <v>0.01144191936627999</v>
       </c>
       <c r="F29">
-        <v>0.003891395678913957</v>
+        <v>0.004313939598655307</v>
       </c>
       <c r="G29">
-        <v>0.001618482664184827</v>
+        <v>0.01145938731186543</v>
       </c>
       <c r="I29">
-        <v>0.001829390214293902</v>
+        <v>0.0113520511070633</v>
       </c>
       <c r="J29">
-        <v>0.002736921514177506</v>
+        <v>-0.01159819825167485</v>
       </c>
       <c r="K29">
-        <v>-0.001665123292651233</v>
+        <v>-0.01144292176473315</v>
       </c>
       <c r="L29">
-        <v>-0.001665123292651233</v>
+        <v>-0.01144292176473315</v>
       </c>
       <c r="O29">
-        <v>-0.001665123292651233</v>
+        <v>-0.01144292176473315</v>
       </c>
       <c r="P29">
-        <v>-0.001613021860130218</v>
+        <v>-0.01146286630410729</v>
       </c>
       <c r="Q29">
-        <v>-0.001639257532392575</v>
+        <v>-0.01145648286650755</v>
       </c>
       <c r="R29">
-        <v>-0.001639257532392575</v>
+        <v>-0.01145648286650755</v>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -1916,40 +1916,40 @@
         <v>77</v>
       </c>
       <c r="C30">
-        <v>-0.01095548902955489</v>
+        <v>0.02473459583179057</v>
       </c>
       <c r="D30">
-        <v>0.004842115728421158</v>
+        <v>0.00527271484019867</v>
       </c>
       <c r="F30">
-        <v>-0.006923286321232863</v>
+        <v>-0.003706860854794702</v>
       </c>
       <c r="G30">
-        <v>0.001798965221989652</v>
+        <v>-0.001155991377437365</v>
       </c>
       <c r="I30">
-        <v>0.001994068219940683</v>
+        <v>-0.001185216393519006</v>
       </c>
       <c r="J30">
-        <v>0.007036224922380164</v>
+        <v>-0.001690213203175934</v>
       </c>
       <c r="K30">
-        <v>-0.001716728765167288</v>
+        <v>0.001229711456714242</v>
       </c>
       <c r="L30">
-        <v>-0.001716728765167288</v>
+        <v>0.001229711456714242</v>
       </c>
       <c r="O30">
-        <v>-0.001716728765167288</v>
+        <v>0.001229711456714242</v>
       </c>
       <c r="P30">
-        <v>-0.001809245262092453</v>
+        <v>0.00114858686169667</v>
       </c>
       <c r="Q30">
-        <v>-0.001752439073524391</v>
+        <v>0.001202706628167291</v>
       </c>
       <c r="R30">
-        <v>-0.001752439073524391</v>
+        <v>0.001202706628167291</v>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -1960,40 +1960,40 @@
         <v>78</v>
       </c>
       <c r="C31">
-        <v>-0.005876753866767539</v>
+        <v>-0.01459379118115299</v>
       </c>
       <c r="D31">
-        <v>-0.01621171205411712</v>
+        <v>0.001742901050670329</v>
       </c>
       <c r="F31">
-        <v>-0.01224104058241041</v>
+        <v>0.009263527879117623</v>
       </c>
       <c r="G31">
-        <v>-0.007624794412247945</v>
+        <v>0.007554460313350943</v>
       </c>
       <c r="I31">
-        <v>-0.007566174627661747</v>
+        <v>0.007943616428806508</v>
       </c>
       <c r="J31">
-        <v>-0.007177086466493077</v>
+        <v>0.01192607514266768</v>
       </c>
       <c r="K31">
-        <v>0.007643394604433947</v>
+        <v>-0.007558128282158257</v>
       </c>
       <c r="L31">
-        <v>0.007643394604433947</v>
+        <v>-0.007558128282158257</v>
       </c>
       <c r="O31">
-        <v>0.007643394604433947</v>
+        <v>-0.007558128282158257</v>
       </c>
       <c r="P31">
-        <v>0.007617246280172463</v>
+        <v>-0.007543598133493722</v>
       </c>
       <c r="Q31">
-        <v>0.007633755532337556</v>
+        <v>-0.007560343290005365</v>
       </c>
       <c r="R31">
-        <v>0.007633755532337556</v>
+        <v>-0.007560343290005365</v>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -2004,40 +2004,40 @@
         <v>79</v>
       </c>
       <c r="C32">
-        <v>0.006080640456806404</v>
+        <v>0.0004682484213788817</v>
       </c>
       <c r="D32">
-        <v>-0.002000245952002459</v>
+        <v>0.0008118716611229948</v>
       </c>
       <c r="F32">
-        <v>-0.007224030264240303</v>
+        <v>0.002341202778768794</v>
       </c>
       <c r="G32">
-        <v>0.0008710422087104221</v>
+        <v>0.004117119767454997</v>
       </c>
       <c r="I32">
-        <v>0.000789382399893824</v>
+        <v>0.004127431072303611</v>
       </c>
       <c r="J32">
-        <v>0.008056055603086225</v>
+        <v>0.01437264767483342</v>
       </c>
       <c r="K32">
-        <v>-0.0008649681686496817</v>
+        <v>-0.00417728122933252</v>
       </c>
       <c r="L32">
-        <v>-0.0008649681686496817</v>
+        <v>-0.00417728122933252</v>
       </c>
       <c r="O32">
-        <v>-0.0008649681686496817</v>
+        <v>-0.00417728122933252</v>
       </c>
       <c r="P32">
-        <v>-0.0008701761807017618</v>
+        <v>-0.004112704423636007</v>
       </c>
       <c r="Q32">
-        <v>-0.0008705083767050838</v>
+        <v>-0.004149782455465351</v>
       </c>
       <c r="R32">
-        <v>-0.0008705083767050838</v>
+        <v>-0.004149782455465351</v>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -2048,40 +2048,40 @@
         <v>80</v>
       </c>
       <c r="C33">
-        <v>0.009066014466660144</v>
+        <v>-0.01285188352893568</v>
       </c>
       <c r="D33">
-        <v>0.003653658888536589</v>
+        <v>-0.005672794541762415</v>
       </c>
       <c r="F33">
-        <v>-0.01440284863202848</v>
+        <v>-0.01076980814484075</v>
       </c>
       <c r="G33">
-        <v>-0.006385750479857504</v>
+        <v>-0.01134346196630409</v>
       </c>
       <c r="I33">
-        <v>-0.006636242874362428</v>
+        <v>-0.01111174892362108</v>
       </c>
       <c r="J33">
-        <v>-0.01216883257100708</v>
+        <v>-0.001659740268162039</v>
       </c>
       <c r="K33">
-        <v>0.006439548508395485</v>
+        <v>0.01136417084944017</v>
       </c>
       <c r="L33">
-        <v>0.006439548508395485</v>
+        <v>0.01136417084944017</v>
       </c>
       <c r="O33">
-        <v>0.006439548508395485</v>
+        <v>0.01136417084944017</v>
       </c>
       <c r="P33">
-        <v>0.006380134647801347</v>
+        <v>0.01134107277095426</v>
       </c>
       <c r="Q33">
-        <v>0.006427958584279586</v>
+        <v>0.01136464869319764</v>
       </c>
       <c r="R33">
-        <v>0.006427958584279586</v>
+        <v>0.01136464869319764</v>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -2092,40 +2092,40 @@
         <v>81</v>
       </c>
       <c r="C34">
-        <v>-0.0122299503862995</v>
+        <v>0.01150871260951114</v>
       </c>
       <c r="D34">
-        <v>-0.00284086194440862</v>
+        <v>0.00213115580673681</v>
       </c>
       <c r="F34">
-        <v>-0.001722985697229857</v>
+        <v>-0.01588750402949225</v>
       </c>
       <c r="G34">
-        <v>0.001495053194950532</v>
+        <v>-0.002712560667383761</v>
       </c>
       <c r="I34">
-        <v>0.001731148865311489</v>
+        <v>-0.002747312972614265</v>
       </c>
       <c r="J34">
-        <v>0.003332264789488134</v>
+        <v>-0.005336442343721514</v>
       </c>
       <c r="K34">
-        <v>-0.001463394422633944</v>
+        <v>0.002799820426559695</v>
       </c>
       <c r="L34">
-        <v>-0.001463394422633944</v>
+        <v>0.002799820426559695</v>
       </c>
       <c r="O34">
-        <v>-0.001463394422633944</v>
+        <v>0.002799820426559695</v>
       </c>
       <c r="P34">
-        <v>-0.0014880699628807</v>
+        <v>0.002704439971944375</v>
       </c>
       <c r="Q34">
-        <v>-0.001471327106713271</v>
+        <v>0.002762121675970652</v>
       </c>
       <c r="R34">
-        <v>-0.001471327106713271</v>
+        <v>0.002762121675970652</v>
       </c>
     </row>
     <row r="35" spans="1:18">
@@ -2136,40 +2136,40 @@
         <v>82</v>
       </c>
       <c r="C35">
-        <v>0.00571469690114697</v>
+        <v>-0.01327153834799279</v>
       </c>
       <c r="D35">
-        <v>0.006341509179415093</v>
+        <v>-0.02401827414872304</v>
       </c>
       <c r="F35">
-        <v>0.02562687367626874</v>
+        <v>-0.01031039657516245</v>
       </c>
       <c r="G35">
-        <v>0.006941301021413011</v>
+        <v>-0.01068515639351807</v>
       </c>
       <c r="I35">
-        <v>0.007089926482899265</v>
+        <v>-0.01044441550694399</v>
       </c>
       <c r="J35">
-        <v>-0.002206691211302949</v>
+        <v>0.02046470522776142</v>
       </c>
       <c r="K35">
-        <v>-0.007073944618739446</v>
+        <v>0.01069990073749845</v>
       </c>
       <c r="L35">
-        <v>-0.007073944618739446</v>
+        <v>0.01069990073749845</v>
       </c>
       <c r="O35">
-        <v>-0.007073944618739446</v>
+        <v>0.01069990073749845</v>
       </c>
       <c r="P35">
-        <v>-0.006930032385300324</v>
+        <v>0.01069069204985456</v>
       </c>
       <c r="Q35">
-        <v>-0.007022542258225422</v>
+        <v>0.01070000233906254</v>
       </c>
       <c r="R35">
-        <v>-0.007022542258225422</v>
+        <v>0.01070000233906254</v>
       </c>
     </row>
     <row r="36" spans="1:18">
@@ -2180,40 +2180,40 @@
         <v>83</v>
       </c>
       <c r="C36">
-        <v>0.003641439168414392</v>
+        <v>-0.006992476374882445</v>
       </c>
       <c r="D36">
-        <v>-0.00246730699267307</v>
+        <v>-0.01595291422582679</v>
       </c>
       <c r="F36">
-        <v>-0.007362197197621972</v>
+        <v>-0.00270055098750861</v>
       </c>
       <c r="G36">
-        <v>-0.001408397858083978</v>
+        <v>-0.004386245810722591</v>
       </c>
       <c r="I36">
-        <v>-0.00147308903073089</v>
+        <v>-0.00461160822830638</v>
       </c>
       <c r="J36">
-        <v>0.005974724762219042</v>
+        <v>-0.0161631960417186</v>
       </c>
       <c r="K36">
-        <v>0.001438662746386627</v>
+        <v>0.004373968896468265</v>
       </c>
       <c r="L36">
-        <v>0.001438662746386627</v>
+        <v>0.004373968896468265</v>
       </c>
       <c r="O36">
-        <v>0.001438662746386627</v>
+        <v>0.004373968896468265</v>
       </c>
       <c r="P36">
-        <v>0.001410818894108189</v>
+        <v>0.004385512709148637</v>
       </c>
       <c r="Q36">
-        <v>0.001422742538227425</v>
+        <v>0.004396129498377024</v>
       </c>
       <c r="R36">
-        <v>0.001422742538227425</v>
+        <v>0.004396129498377024</v>
       </c>
     </row>
     <row r="37" spans="1:18">
@@ -2224,40 +2224,40 @@
         <v>83</v>
       </c>
       <c r="C37">
-        <v>0.01266725065867251</v>
+        <v>0.006302324278161318</v>
       </c>
       <c r="D37">
-        <v>-0.01519095769990958</v>
+        <v>-0.004795681270245021</v>
       </c>
       <c r="F37">
-        <v>-0.007181248763812488</v>
+        <v>0.00112544769727262</v>
       </c>
       <c r="G37">
-        <v>-0.008458565796585658</v>
+        <v>0.001662746299417911</v>
       </c>
       <c r="I37">
-        <v>-0.008833836568338365</v>
+        <v>0.001443385920990405</v>
       </c>
       <c r="J37">
-        <v>-0.009047995112600469</v>
+        <v>-0.004161539480047146</v>
       </c>
       <c r="K37">
-        <v>0.00846718492867185</v>
+        <v>-0.001685657674775902</v>
       </c>
       <c r="L37">
-        <v>0.00846718492867185</v>
+        <v>-0.001685657674775902</v>
       </c>
       <c r="O37">
-        <v>0.00846718492867185</v>
+        <v>-0.001685657674775902</v>
       </c>
       <c r="P37">
-        <v>0.008457722136577223</v>
+        <v>-0.001662771072855798</v>
       </c>
       <c r="Q37">
-        <v>0.008460940740609407</v>
+        <v>-0.001678808604356385</v>
       </c>
       <c r="R37">
-        <v>0.008460940740609407</v>
+        <v>-0.001678808604356385</v>
       </c>
     </row>
     <row r="38" spans="1:18">
@@ -2268,40 +2268,40 @@
         <v>83</v>
       </c>
       <c r="C38">
-        <v>-0.01949335771493358</v>
+        <v>0.007456919975889376</v>
       </c>
       <c r="D38">
-        <v>-0.01165142259251423</v>
+        <v>0.01924398648818729</v>
       </c>
       <c r="F38">
-        <v>-0.001929280735292807</v>
+        <v>0.005349402294521912</v>
       </c>
       <c r="G38">
-        <v>-0.001505894427058944</v>
+        <v>0.01313096465048382</v>
       </c>
       <c r="I38">
-        <v>-0.001471742186717422</v>
+        <v>0.01310784885324764</v>
       </c>
       <c r="J38">
-        <v>-0.004564813080218349</v>
+        <v>0.00871803603013278</v>
       </c>
       <c r="K38">
-        <v>0.001539550083395501</v>
+        <v>-0.01304327303192614</v>
       </c>
       <c r="L38">
-        <v>0.001539550083395501</v>
+        <v>-0.01304327303192614</v>
       </c>
       <c r="O38">
-        <v>0.001539550083395501</v>
+        <v>-0.01304327303192614</v>
       </c>
       <c r="P38">
-        <v>0.001505677323056773</v>
+        <v>-0.01313916107248689</v>
       </c>
       <c r="Q38">
-        <v>0.001521177303211773</v>
+        <v>-0.0130598463212476</v>
       </c>
       <c r="R38">
-        <v>0.001521177303211773</v>
+        <v>-0.0130598463212476</v>
       </c>
     </row>
     <row r="39" spans="1:18">
@@ -2312,40 +2312,40 @@
         <v>83</v>
       </c>
       <c r="C39">
-        <v>0.01975830402558304</v>
+        <v>-0.001344024817875388</v>
       </c>
       <c r="D39">
-        <v>0.007499023610990236</v>
+        <v>0.01430752569230509</v>
       </c>
       <c r="F39">
-        <v>0.01510101622301016</v>
+        <v>0.002492902749889106</v>
       </c>
       <c r="G39">
-        <v>0.01722618421626184</v>
+        <v>0.0123766206621347</v>
       </c>
       <c r="I39">
-        <v>0.01703988767039888</v>
+        <v>0.01221856718310261</v>
       </c>
       <c r="J39">
-        <v>0.01488420707981582</v>
+        <v>0.01161193778602961</v>
       </c>
       <c r="K39">
-        <v>-0.01725344812053448</v>
+        <v>-0.0123328444505132</v>
       </c>
       <c r="L39">
-        <v>-0.01725344812053448</v>
+        <v>-0.0123328444505132</v>
       </c>
       <c r="O39">
-        <v>-0.01725344812053448</v>
+        <v>-0.0123328444505132</v>
       </c>
       <c r="P39">
-        <v>-0.01722184648021846</v>
+        <v>-0.01238428882631702</v>
       </c>
       <c r="Q39">
-        <v>-0.01723906778839068</v>
+        <v>-0.01234635602884931</v>
       </c>
       <c r="R39">
-        <v>-0.01723906778839068</v>
+        <v>-0.01234635602884931</v>
       </c>
     </row>
     <row r="40" spans="1:18">
@@ -2356,40 +2356,40 @@
         <v>83</v>
       </c>
       <c r="C40">
-        <v>-0.007785020309850203</v>
+        <v>0.001869703740151621</v>
       </c>
       <c r="D40">
-        <v>-0.003414632878146329</v>
+        <v>-0.00962075250969926</v>
       </c>
       <c r="F40">
-        <v>0.009693033564930335</v>
+        <v>-0.01527009776203278</v>
       </c>
       <c r="G40">
-        <v>0.0001213092492130925</v>
+        <v>-0.0209935229061488</v>
       </c>
       <c r="I40">
-        <v>0.000224619506246195</v>
+        <v>-0.0213312509583008</v>
       </c>
       <c r="J40">
-        <v>0.009805627811054242</v>
+        <v>0.007336570237269368</v>
       </c>
       <c r="K40">
-        <v>-0.0001724163737241637</v>
+        <v>0.02101687232838863</v>
       </c>
       <c r="L40">
-        <v>-0.0001724163737241637</v>
+        <v>0.02101687232838863</v>
       </c>
       <c r="O40">
-        <v>-0.0001724163737241637</v>
+        <v>0.02101687232838863</v>
       </c>
       <c r="P40">
-        <v>-0.0001105711931057119</v>
+        <v>0.02100308116411065</v>
       </c>
       <c r="Q40">
-        <v>-0.0001497273134972731</v>
+        <v>0.02101759012527485</v>
       </c>
       <c r="R40">
-        <v>-0.0001497273134972731</v>
+        <v>0.02101759012527485</v>
       </c>
     </row>
     <row r="41" spans="1:18">
@@ -2400,40 +2400,40 @@
         <v>84</v>
       </c>
       <c r="C41">
-        <v>-0.06239567150395671</v>
+        <v>-0.05079881439529398</v>
       </c>
       <c r="D41">
-        <v>-0.0122099903780999</v>
+        <v>0.002546723336667552</v>
       </c>
       <c r="F41">
-        <v>-0.021411699970117</v>
+        <v>0.004700249885941405</v>
       </c>
       <c r="G41">
-        <v>-0.02261542238215422</v>
+        <v>0.00279959230936863</v>
       </c>
       <c r="I41">
-        <v>-0.02288224132882241</v>
+        <v>0.002828092497313946</v>
       </c>
       <c r="J41">
-        <v>-0.003792566591361009</v>
+        <v>0.01359444890835017</v>
       </c>
       <c r="K41">
-        <v>0.02267330498273305</v>
+        <v>-0.002850690747667044</v>
       </c>
       <c r="L41">
-        <v>0.02267330498273305</v>
+        <v>-0.002850690747667044</v>
       </c>
       <c r="O41">
-        <v>0.02267330498273305</v>
+        <v>-0.002850690747667044</v>
       </c>
       <c r="P41">
-        <v>0.02260712492207125</v>
+        <v>-0.002788287207629488</v>
       </c>
       <c r="Q41">
-        <v>0.02265177166651771</v>
+        <v>-0.002834539895852186</v>
       </c>
       <c r="R41">
-        <v>0.02265177166651771</v>
+        <v>-0.002834539895852186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>